<commit_message>
began pattern testing for health & species prevalency
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-Toolbox\fmgpy\summaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FF073D-C833-4F7B-BF02-C505B2CE3812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCD2DA6-BFBB-4E6E-96BC-692B2B1B154A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="One To One" sheetId="1" r:id="rId1"/>
@@ -2156,9 +2156,6 @@
     <t>forest_calcs.TPA_BA_QMDBH_Plot &amp; Level</t>
   </si>
   <si>
-    <t>forest_calcs.create_general_description_level</t>
-  </si>
-  <si>
     <t>Total Number of Age Trees</t>
   </si>
   <si>
@@ -2172,6 +2169,9 @@
   </si>
   <si>
     <t>Age Tree Average Diameter</t>
+  </si>
+  <si>
+    <t>01_general_description_summary - plot &amp; level</t>
   </si>
 </sst>
 </file>
@@ -2792,26 +2792,26 @@
   <dimension ref="A1:L223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E240" sqref="E240"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" customWidth="1"/>
+    <col min="3" max="3" width="41.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="51.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.42578125" customWidth="1"/>
-    <col min="9" max="9" width="59.85546875" customWidth="1"/>
-    <col min="10" max="10" width="53.140625" customWidth="1"/>
-    <col min="11" max="11" width="32.5703125" customWidth="1"/>
-    <col min="12" max="12" width="91.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.453125" customWidth="1"/>
+    <col min="9" max="9" width="59.81640625" customWidth="1"/>
+    <col min="10" max="10" width="53.1796875" customWidth="1"/>
+    <col min="11" max="11" width="32.54296875" customWidth="1"/>
+    <col min="12" max="12" width="91.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2857,13 +2857,13 @@
         <v>592</v>
       </c>
       <c r="C2" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -2881,7 +2881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2889,13 +2889,13 @@
         <v>592</v>
       </c>
       <c r="C3" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -2913,21 +2913,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>601</v>
+      <c r="C4" t="s">
+        <v>606</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>17</v>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2955,13 +2955,13 @@
         <v>592</v>
       </c>
       <c r="C5" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -2982,21 +2982,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>601</v>
+      <c r="C6" t="s">
+        <v>606</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>24</v>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3026,13 +3026,13 @@
         <v>592</v>
       </c>
       <c r="C7" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>28</v>
@@ -3053,7 +3053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3079,7 +3079,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3087,13 +3087,13 @@
         <v>592</v>
       </c>
       <c r="C9" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
@@ -3114,21 +3114,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>601</v>
+      <c r="C10" t="s">
+        <v>606</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>40</v>
@@ -3150,21 +3150,21 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>601</v>
+      <c r="C11" t="s">
+        <v>606</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>595</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>45</v>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3194,13 +3194,13 @@
         <v>592</v>
       </c>
       <c r="C12" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D12" t="s">
         <v>596</v>
       </c>
       <c r="E12" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F12" t="s">
         <v>49</v>
@@ -3221,7 +3221,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3229,16 +3229,16 @@
         <v>592</v>
       </c>
       <c r="C13" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F13" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G13" t="s">
         <v>53</v>
@@ -3256,7 +3256,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3264,13 +3264,13 @@
         <v>592</v>
       </c>
       <c r="C14" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F14" t="s">
         <v>56</v>
@@ -3288,21 +3288,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>601</v>
+      <c r="C15" s="2" t="s">
+        <v>606</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>462</v>
@@ -3322,21 +3322,21 @@
       </c>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>601</v>
+      <c r="C16" t="s">
+        <v>606</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>59</v>
@@ -3356,21 +3356,21 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>601</v>
+      <c r="C17" s="2" t="s">
+        <v>606</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>463</v>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3398,13 +3398,13 @@
         <v>592</v>
       </c>
       <c r="C18" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F18" t="s">
         <v>61</v>
@@ -3422,21 +3422,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>601</v>
+      <c r="C19" s="2" t="s">
+        <v>606</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>464</v>
@@ -3456,21 +3456,21 @@
       </c>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>601</v>
+      <c r="C20" t="s">
+        <v>606</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>470</v>
@@ -3492,7 +3492,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3500,13 +3500,13 @@
         <v>592</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>471</v>
@@ -3527,21 +3527,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>601</v>
+      <c r="C22" s="2" t="s">
+        <v>606</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>465</v>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>64</v>
       </c>
@@ -3650,7 +3650,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>53</v>
@@ -3669,7 +3669,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3677,13 +3677,13 @@
         <v>592</v>
       </c>
       <c r="C28" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D28" t="s">
         <v>595</v>
       </c>
       <c r="E28" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F28" t="s">
         <v>70</v>
@@ -3707,7 +3707,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3715,13 +3715,13 @@
         <v>592</v>
       </c>
       <c r="C29" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D29" t="s">
         <v>595</v>
       </c>
       <c r="E29" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F29" t="s">
         <v>75</v>
@@ -3745,7 +3745,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -3753,13 +3753,13 @@
         <v>592</v>
       </c>
       <c r="C30" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D30" t="s">
         <v>595</v>
       </c>
       <c r="E30" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>80</v>
@@ -3783,7 +3783,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -3791,13 +3791,13 @@
         <v>592</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>595</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>458</v>
@@ -3821,21 +3821,21 @@
         <v>460</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>601</v>
+      <c r="C32" s="2" t="s">
+        <v>606</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>595</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>478</v>
@@ -3857,7 +3857,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>85</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>85</v>
       </c>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>85</v>
       </c>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>85</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>85</v>
       </c>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>85</v>
       </c>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>85</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>85</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>85</v>
       </c>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>85</v>
       </c>
@@ -4720,7 +4720,7 @@
       </c>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>85</v>
       </c>
@@ -4748,7 +4748,7 @@
       </c>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>85</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>85</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>85</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>85</v>
       </c>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>85</v>
       </c>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>85</v>
       </c>
@@ -5403,7 +5403,7 @@
       </c>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>85</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>595</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>518</v>
@@ -5555,7 +5555,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>85</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>595</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>519</v>
@@ -5593,7 +5593,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>85</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>595</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>520</v>
@@ -5631,7 +5631,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>85</v>
       </c>
@@ -5659,7 +5659,7 @@
       </c>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>85</v>
       </c>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>85</v>
       </c>
@@ -5715,7 +5715,7 @@
       </c>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>85</v>
       </c>
@@ -5743,7 +5743,7 @@
       </c>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>85</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>596</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>525</v>
@@ -5781,7 +5781,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>85</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>596</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>526</v>
@@ -5819,7 +5819,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>85</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>596</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>527</v>
@@ -5857,7 +5857,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>185</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>185</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>185</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>185</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>185</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>185</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>185</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>185</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>185</v>
       </c>
@@ -6182,7 +6182,7 @@
       </c>
       <c r="L102" s="5"/>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>185</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>185</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>185</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>185</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="107" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>185</v>
       </c>
@@ -6342,7 +6342,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>185</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>185</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>185</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>185</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>185</v>
       </c>
@@ -6507,7 +6507,7 @@
       </c>
       <c r="L112" s="5"/>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>185</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>224</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>224</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>224</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>224</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="118" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>224</v>
       </c>
@@ -6693,7 +6693,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>224</v>
       </c>
@@ -6721,7 +6721,7 @@
       </c>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>224</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>224</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>224</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>224</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>224</v>
       </c>
@@ -6886,7 +6886,7 @@
       </c>
       <c r="L124" s="4"/>
     </row>
-    <row r="125" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>224</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>224</v>
       </c>
@@ -6937,7 +6937,7 @@
       </c>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>224</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>224</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>224</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>224</v>
       </c>
@@ -7074,7 +7074,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>224</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="132" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>224</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>224</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="134" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>224</v>
       </c>
@@ -7171,7 +7171,7 @@
       </c>
       <c r="L134" s="5"/>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>224</v>
       </c>
@@ -7209,7 +7209,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>224</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>224</v>
       </c>
@@ -7285,7 +7285,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>224</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="139" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>224</v>
       </c>
@@ -7336,7 +7336,7 @@
       </c>
       <c r="L139" s="5"/>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>224</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="141" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>224</v>
       </c>
@@ -7387,7 +7387,7 @@
       </c>
       <c r="L141" s="5"/>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>272</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>272</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>272</v>
       </c>
@@ -7456,7 +7456,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>272</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>272</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>272</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>272</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>272</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>272</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>272</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>272</v>
       </c>
@@ -7649,7 +7649,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>272</v>
       </c>
@@ -7675,7 +7675,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>272</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>272</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>272</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>272</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="4" t="s">
         <v>272</v>
       </c>
@@ -7804,7 +7804,7 @@
       </c>
       <c r="L158" s="4"/>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
         <v>272</v>
       </c>
@@ -7834,7 +7834,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>272</v>
       </c>
@@ -7862,7 +7862,7 @@
       </c>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>272</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>272</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>272</v>
       </c>
@@ -7940,7 +7940,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
         <v>272</v>
       </c>
@@ -7968,7 +7968,7 @@
       </c>
       <c r="L164" s="4"/>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>272</v>
       </c>
@@ -7994,7 +7994,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
         <v>272</v>
       </c>
@@ -8022,7 +8022,7 @@
       </c>
       <c r="L166" s="4"/>
     </row>
-    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>272</v>
       </c>
@@ -8048,7 +8048,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>272</v>
       </c>
@@ -8078,7 +8078,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>272</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" s="4" t="s">
         <v>272</v>
       </c>
@@ -8132,7 +8132,7 @@
       </c>
       <c r="L170" s="4"/>
     </row>
-    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>272</v>
       </c>
@@ -8158,7 +8158,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
         <v>272</v>
       </c>
@@ -8186,7 +8186,7 @@
       </c>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>272</v>
       </c>
@@ -8212,7 +8212,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
         <v>272</v>
       </c>
@@ -8242,7 +8242,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>272</v>
       </c>
@@ -8268,7 +8268,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
         <v>272</v>
       </c>
@@ -8296,7 +8296,7 @@
       </c>
       <c r="L176" s="4"/>
     </row>
-    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>272</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>368</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
         <v>368</v>
       </c>
@@ -8378,7 +8378,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>64</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>64</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>383</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="183" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>383</v>
       </c>
@@ -8473,7 +8473,7 @@
       </c>
       <c r="L183" s="5"/>
     </row>
-    <row r="184" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
         <v>383</v>
       </c>
@@ -8497,7 +8497,7 @@
       <c r="K184" s="5"/>
       <c r="L184" s="5"/>
     </row>
-    <row r="185" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>383</v>
       </c>
@@ -8519,21 +8519,21 @@
       <c r="K185" s="5"/>
       <c r="L185" s="5"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B186" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="C186" s="4" t="s">
-        <v>601</v>
+      <c r="C186" t="s">
+        <v>606</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F186" s="4" t="s">
         <v>389</v>
@@ -8555,7 +8555,7 @@
       </c>
       <c r="L186" s="4"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -8563,13 +8563,13 @@
         <v>592</v>
       </c>
       <c r="C187" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D187" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E187" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F187" t="s">
         <v>393</v>
@@ -8590,7 +8590,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>185</v>
       </c>
@@ -8613,7 +8613,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="189" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
         <v>185</v>
       </c>
@@ -8641,7 +8641,7 @@
       </c>
       <c r="L189" s="5"/>
     </row>
-    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>185</v>
       </c>
@@ -8664,7 +8664,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="191" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
         <v>185</v>
       </c>
@@ -8687,7 +8687,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>185</v>
       </c>
@@ -8710,7 +8710,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="193" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
         <v>185</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>185</v>
       </c>
@@ -8756,7 +8756,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="195" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>185</v>
       </c>
@@ -8784,7 +8784,7 @@
       </c>
       <c r="L195" s="5"/>
     </row>
-    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>185</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="197" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
         <v>185</v>
       </c>
@@ -8835,7 +8835,7 @@
       </c>
       <c r="L197" s="5"/>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>185</v>
       </c>
@@ -8858,7 +8858,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="199" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>185</v>
       </c>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="L199" s="5"/>
     </row>
-    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" s="4" t="s">
         <v>426</v>
       </c>
@@ -8914,7 +8914,7 @@
       </c>
       <c r="L200" s="4"/>
     </row>
-    <row r="201" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
         <v>426</v>
       </c>
@@ -8937,7 +8937,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" s="4" t="s">
         <v>426</v>
       </c>
@@ -8965,7 +8965,7 @@
       </c>
       <c r="L202" s="4"/>
     </row>
-    <row r="203" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
         <v>426</v>
       </c>
@@ -8988,7 +8988,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="204" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
         <v>426</v>
       </c>
@@ -9026,7 +9026,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="205" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
         <v>426</v>
       </c>
@@ -9064,7 +9064,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="206" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
         <v>426</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="207" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
         <v>426</v>
       </c>
@@ -9140,7 +9140,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="208" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" s="2" t="s">
         <v>426</v>
       </c>
@@ -9178,7 +9178,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="209" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" s="2" t="s">
         <v>426</v>
       </c>
@@ -9216,7 +9216,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="210" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" s="2" t="s">
         <v>426</v>
       </c>
@@ -9239,7 +9239,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="211" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
         <v>426</v>
       </c>
@@ -9262,7 +9262,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="212" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
         <v>426</v>
       </c>
@@ -9285,7 +9285,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="213" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
         <v>426</v>
       </c>
@@ -9308,7 +9308,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="214" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
         <v>426</v>
       </c>
@@ -9331,7 +9331,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="215" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
         <v>426</v>
       </c>
@@ -9369,7 +9369,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="216" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>426</v>
       </c>
@@ -9407,7 +9407,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="217" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>426</v>
       </c>
@@ -9445,7 +9445,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="218" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" s="5" t="s">
         <v>426</v>
       </c>
@@ -9483,7 +9483,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="219" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" s="5" t="s">
         <v>426</v>
       </c>
@@ -9521,7 +9521,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="220" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
         <v>426</v>
       </c>
@@ -9559,7 +9559,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>8</v>
       </c>
@@ -9567,13 +9567,13 @@
         <v>592</v>
       </c>
       <c r="C221" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D221" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E221" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F221" t="s">
         <v>417</v>
@@ -9594,7 +9594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>8</v>
       </c>
@@ -9602,13 +9602,13 @@
         <v>592</v>
       </c>
       <c r="C222" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D222" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E222" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F222" t="s">
         <v>420</v>
@@ -9629,7 +9629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>368</v>
       </c>
@@ -9656,7 +9656,7 @@
   <autoFilter ref="A1:L223" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
     <filterColumn colId="0">
       <filters>
-        <filter val="General Descriptive"/>
+        <filter val="Health"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -9674,19 +9674,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="32.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.453125" customWidth="1"/>
+    <col min="7" max="7" width="31.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9712,12 +9712,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>587</v>
       </c>

</xml_diff>

<commit_message>
continued debug of health prevalence
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0303C75-2C2C-47E3-B028-74112CA87425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D07C2D4-9044-4C8C-A6D2-5E4050FA0937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
+    <workbookView xWindow="40080" yWindow="3570" windowWidth="36400" windowHeight="16650" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="One To One" sheetId="1" r:id="rId1"/>
@@ -2782,10 +2782,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K211" sqref="K211"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2842,7 +2843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2874,7 +2875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2906,7 +2907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -2940,7 +2941,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2975,7 +2976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -3011,7 +3012,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3046,7 +3047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3072,7 +3073,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3107,7 +3108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -3143,7 +3144,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -3179,7 +3180,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3214,7 +3215,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3249,7 +3250,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3281,7 +3282,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -3315,7 +3316,7 @@
       </c>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -3349,7 +3350,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -3383,7 +3384,7 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3415,7 +3416,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
@@ -3449,7 +3450,7 @@
       </c>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
@@ -3485,7 +3486,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3520,7 +3521,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -3554,7 +3555,7 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3574,7 +3575,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3594,7 +3595,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3614,7 +3615,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -3634,7 +3635,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>64</v>
       </c>
@@ -3662,7 +3663,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3700,7 +3701,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3738,7 +3739,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -3776,7 +3777,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -3814,7 +3815,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
@@ -3850,7 +3851,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>85</v>
       </c>
@@ -3888,7 +3889,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -3926,7 +3927,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -4015,7 +4016,7 @@
       </c>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
@@ -4043,7 +4044,7 @@
       </c>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>85</v>
       </c>
@@ -4071,7 +4072,7 @@
       </c>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -4109,7 +4110,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -4147,7 +4148,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -4185,7 +4186,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -4223,7 +4224,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>85</v>
       </c>
@@ -4261,7 +4262,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -4355,7 +4356,7 @@
       </c>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -4378,7 +4379,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -4406,7 +4407,7 @@
       </c>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -4444,7 +4445,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>85</v>
       </c>
@@ -4482,7 +4483,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -4520,7 +4521,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>85</v>
       </c>
@@ -4558,7 +4559,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -4596,7 +4597,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -4685,7 +4686,7 @@
       </c>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>85</v>
       </c>
@@ -4713,7 +4714,7 @@
       </c>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>85</v>
       </c>
@@ -4741,7 +4742,7 @@
       </c>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>85</v>
       </c>
@@ -4779,7 +4780,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -4817,7 +4818,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -4855,7 +4856,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -4893,7 +4894,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -4931,7 +4932,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>85</v>
       </c>
@@ -5015,7 +5016,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -5038,7 +5039,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>85</v>
       </c>
@@ -5066,7 +5067,7 @@
       </c>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -5104,7 +5105,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -5142,7 +5143,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -5180,7 +5181,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -5218,7 +5219,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -5256,7 +5257,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -5345,7 +5346,7 @@
       </c>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -5368,7 +5369,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>85</v>
       </c>
@@ -5396,7 +5397,7 @@
       </c>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -5434,7 +5435,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -5472,7 +5473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -5510,7 +5511,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>85</v>
       </c>
@@ -5548,7 +5549,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>85</v>
       </c>
@@ -5586,7 +5587,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>85</v>
       </c>
@@ -5680,7 +5681,7 @@
       </c>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>85</v>
       </c>
@@ -5708,7 +5709,7 @@
       </c>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>85</v>
       </c>
@@ -5736,7 +5737,7 @@
       </c>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>85</v>
       </c>
@@ -5774,7 +5775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>85</v>
       </c>
@@ -5812,7 +5813,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>85</v>
       </c>
@@ -5850,7 +5851,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>183</v>
       </c>
@@ -5888,7 +5889,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -5926,7 +5927,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>183</v>
       </c>
@@ -5964,7 +5965,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>183</v>
       </c>
@@ -5987,7 +5988,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="97" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>183</v>
       </c>
@@ -6010,7 +6011,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>183</v>
       </c>
@@ -6048,7 +6049,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>183</v>
       </c>
@@ -6086,7 +6087,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>183</v>
       </c>
@@ -6124,7 +6125,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>183</v>
       </c>
@@ -6147,7 +6148,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="102" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>183</v>
       </c>
@@ -6175,7 +6176,7 @@
       </c>
       <c r="L102" s="5"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>183</v>
       </c>
@@ -6213,7 +6214,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>183</v>
       </c>
@@ -6251,7 +6252,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>183</v>
       </c>
@@ -6289,7 +6290,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>183</v>
       </c>
@@ -6312,7 +6313,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="107" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>183</v>
       </c>
@@ -6335,7 +6336,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>183</v>
       </c>
@@ -6373,7 +6374,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>183</v>
       </c>
@@ -6411,7 +6412,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>183</v>
       </c>
@@ -6449,7 +6450,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>183</v>
       </c>
@@ -6472,7 +6473,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="112" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>183</v>
       </c>
@@ -6500,7 +6501,7 @@
       </c>
       <c r="L112" s="5"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>183</v>
       </c>
@@ -6526,7 +6527,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>222</v>
       </c>
@@ -6564,7 +6565,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>222</v>
       </c>
@@ -6602,7 +6603,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>222</v>
       </c>
@@ -6686,7 +6687,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>222</v>
       </c>
@@ -6714,7 +6715,7 @@
       </c>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>222</v>
       </c>
@@ -6737,7 +6738,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>222</v>
       </c>
@@ -6775,7 +6776,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>222</v>
       </c>
@@ -6813,7 +6814,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>222</v>
       </c>
@@ -6902,7 +6903,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>222</v>
       </c>
@@ -6930,7 +6931,7 @@
       </c>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>222</v>
       </c>
@@ -6953,7 +6954,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>222</v>
       </c>
@@ -6991,7 +6992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>222</v>
       </c>
@@ -7029,7 +7030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>222</v>
       </c>
@@ -7113,7 +7114,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>222</v>
       </c>
@@ -7136,7 +7137,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="134" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>222</v>
       </c>
@@ -7164,7 +7165,7 @@
       </c>
       <c r="L134" s="5"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>222</v>
       </c>
@@ -7202,7 +7203,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>222</v>
       </c>
@@ -7240,7 +7241,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>222</v>
       </c>
@@ -7329,7 +7330,7 @@
       </c>
       <c r="L139" s="5"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>222</v>
       </c>
@@ -7352,7 +7353,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="141" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>222</v>
       </c>
@@ -7380,7 +7381,7 @@
       </c>
       <c r="L141" s="5"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>270</v>
       </c>
@@ -7403,7 +7404,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>270</v>
       </c>
@@ -7426,7 +7427,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>270</v>
       </c>
@@ -7449,7 +7450,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>270</v>
       </c>
@@ -7472,7 +7473,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>270</v>
       </c>
@@ -7495,7 +7496,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>270</v>
       </c>
@@ -7518,7 +7519,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>270</v>
       </c>
@@ -7541,7 +7542,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>270</v>
       </c>
@@ -7567,7 +7568,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>270</v>
       </c>
@@ -7593,7 +7594,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>270</v>
       </c>
@@ -7668,7 +7669,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>270</v>
       </c>
@@ -7691,7 +7692,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>270</v>
       </c>
@@ -7717,7 +7718,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>270</v>
       </c>
@@ -7743,7 +7744,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>270</v>
       </c>
@@ -7827,7 +7828,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>270</v>
       </c>
@@ -7855,7 +7856,7 @@
       </c>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>270</v>
       </c>
@@ -7881,7 +7882,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>270</v>
       </c>
@@ -7907,7 +7908,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>270</v>
       </c>
@@ -7987,7 +7988,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
         <v>270</v>
       </c>
@@ -8015,7 +8016,7 @@
       </c>
       <c r="L166" s="4"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>270</v>
       </c>
@@ -8041,7 +8042,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>270</v>
       </c>
@@ -8071,7 +8072,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>270</v>
       </c>
@@ -8151,7 +8152,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
         <v>270</v>
       </c>
@@ -8179,7 +8180,7 @@
       </c>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>270</v>
       </c>
@@ -8205,7 +8206,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
         <v>270</v>
       </c>
@@ -8235,7 +8236,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>270</v>
       </c>
@@ -8315,7 +8316,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>364</v>
       </c>
@@ -8341,7 +8342,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
         <v>364</v>
       </c>
@@ -8371,7 +8372,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>64</v>
       </c>
@@ -8394,7 +8395,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>64</v>
       </c>
@@ -8417,7 +8418,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>379</v>
       </c>
@@ -8440,7 +8441,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="183" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>379</v>
       </c>
@@ -8466,7 +8467,7 @@
       </c>
       <c r="L183" s="5"/>
     </row>
-    <row r="184" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
         <v>379</v>
       </c>
@@ -8490,7 +8491,7 @@
       <c r="K184" s="5"/>
       <c r="L184" s="5"/>
     </row>
-    <row r="185" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>379</v>
       </c>
@@ -8512,7 +8513,7 @@
       <c r="K185" s="5"/>
       <c r="L185" s="5"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="4" t="s">
         <v>8</v>
       </c>
@@ -8548,7 +8549,7 @@
       </c>
       <c r="L186" s="4"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -8634,7 +8635,7 @@
       </c>
       <c r="L189" s="5"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>183</v>
       </c>
@@ -8657,7 +8658,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="191" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
         <v>183</v>
       </c>
@@ -8726,7 +8727,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>183</v>
       </c>
@@ -8749,7 +8750,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="195" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>183</v>
       </c>
@@ -8828,7 +8829,7 @@
       </c>
       <c r="L197" s="5"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>183</v>
       </c>
@@ -8851,7 +8852,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="199" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>183</v>
       </c>
@@ -8930,7 +8931,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" s="4" t="s">
         <v>422</v>
       </c>
@@ -8958,7 +8959,7 @@
       </c>
       <c r="L202" s="4"/>
     </row>
-    <row r="203" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
         <v>422</v>
       </c>
@@ -8981,7 +8982,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="204" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
         <v>422</v>
       </c>
@@ -9019,7 +9020,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="205" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
         <v>422</v>
       </c>
@@ -9057,7 +9058,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="206" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
         <v>422</v>
       </c>
@@ -9095,7 +9096,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="207" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
         <v>422</v>
       </c>
@@ -9133,7 +9134,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="208" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" s="2" t="s">
         <v>422</v>
       </c>
@@ -9171,7 +9172,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="209" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" s="2" t="s">
         <v>422</v>
       </c>
@@ -9232,7 +9233,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="211" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
         <v>422</v>
       </c>
@@ -9255,7 +9256,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="212" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
         <v>422</v>
       </c>
@@ -9278,7 +9279,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="213" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
         <v>422</v>
       </c>
@@ -9301,7 +9302,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="214" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
         <v>422</v>
       </c>
@@ -9324,7 +9325,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="215" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
         <v>422</v>
       </c>
@@ -9362,7 +9363,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="216" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>422</v>
       </c>
@@ -9400,7 +9401,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="217" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>422</v>
       </c>
@@ -9438,7 +9439,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="218" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" s="5" t="s">
         <v>422</v>
       </c>
@@ -9476,7 +9477,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="219" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" s="5" t="s">
         <v>422</v>
       </c>
@@ -9514,7 +9515,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="220" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
         <v>422</v>
       </c>
@@ -9552,7 +9553,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>8</v>
       </c>
@@ -9587,7 +9588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>8</v>
       </c>
@@ -9622,7 +9623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>364</v>
       </c>
@@ -9646,7 +9647,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L223" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}"/>
+  <autoFilter ref="A1:L223" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="Health Prevalency by TPA"/>
+        <filter val="Health Prevalency Percentage"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
continue debug health summary
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-toolbox\fmgpy\summaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-Toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D07C2D4-9044-4C8C-A6D2-5E4050FA0937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1139D15-4B7B-4B57-8938-9D4E349279E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40080" yWindow="3570" windowWidth="36400" windowHeight="16650" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="One To One" sheetId="1" r:id="rId1"/>
@@ -2786,26 +2786,26 @@
   <dimension ref="A1:L223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F210" sqref="F210"/>
+      <selection activeCell="D228" sqref="D228"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" customWidth="1"/>
-    <col min="2" max="2" width="25.81640625" customWidth="1"/>
-    <col min="3" max="3" width="41.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="51.453125" customWidth="1"/>
-    <col min="7" max="7" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.453125" customWidth="1"/>
-    <col min="9" max="9" width="59.81640625" customWidth="1"/>
-    <col min="10" max="10" width="53.1796875" customWidth="1"/>
-    <col min="11" max="11" width="32.54296875" customWidth="1"/>
-    <col min="12" max="12" width="91.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.42578125" customWidth="1"/>
+    <col min="9" max="9" width="59.85546875" customWidth="1"/>
+    <col min="10" max="10" width="53.140625" customWidth="1"/>
+    <col min="11" max="11" width="32.5703125" customWidth="1"/>
+    <col min="12" max="12" width="91.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -3144,7 +3144,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -3316,7 +3316,7 @@
       </c>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -3350,7 +3350,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -3384,7 +3384,7 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
@@ -3486,7 +3486,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -3555,7 +3555,7 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>64</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>85</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>85</v>
       </c>
@@ -4016,7 +4016,7 @@
       </c>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
@@ -4044,7 +4044,7 @@
       </c>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>85</v>
       </c>
@@ -4072,7 +4072,7 @@
       </c>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>85</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>85</v>
       </c>
@@ -4328,7 +4328,7 @@
       </c>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>85</v>
       </c>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -4407,7 +4407,7 @@
       </c>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>85</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>85</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>85</v>
       </c>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>85</v>
       </c>
@@ -4714,7 +4714,7 @@
       </c>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>85</v>
       </c>
@@ -4742,7 +4742,7 @@
       </c>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>85</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -4932,7 +4932,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>85</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>85</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>85</v>
       </c>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="77" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>85</v>
       </c>
@@ -5346,7 +5346,7 @@
       </c>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>85</v>
       </c>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>85</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>85</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>85</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>85</v>
       </c>
@@ -5653,7 +5653,7 @@
       </c>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>85</v>
       </c>
@@ -5681,7 +5681,7 @@
       </c>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>85</v>
       </c>
@@ -5709,7 +5709,7 @@
       </c>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>85</v>
       </c>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>85</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>85</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>85</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>183</v>
       </c>
@@ -5889,7 +5889,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -5927,7 +5927,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>183</v>
       </c>
@@ -5965,7 +5965,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>183</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="97" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>183</v>
       </c>
@@ -6011,7 +6011,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>183</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>183</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>183</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>183</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="102" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>183</v>
       </c>
@@ -6176,7 +6176,7 @@
       </c>
       <c r="L102" s="5"/>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>183</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>183</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>183</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>183</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="107" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>183</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>183</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>183</v>
       </c>
@@ -6412,7 +6412,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>183</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>183</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="112" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>183</v>
       </c>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="L112" s="5"/>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>183</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>222</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>222</v>
       </c>
@@ -6603,7 +6603,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>222</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>222</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="118" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>222</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>222</v>
       </c>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>222</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>222</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>222</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>222</v>
       </c>
@@ -6852,7 +6852,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>222</v>
       </c>
@@ -6880,7 +6880,7 @@
       </c>
       <c r="L124" s="4"/>
     </row>
-    <row r="125" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>222</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>222</v>
       </c>
@@ -6931,7 +6931,7 @@
       </c>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>222</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>222</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>222</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>222</v>
       </c>
@@ -7068,7 +7068,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>222</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="132" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>222</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>222</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="134" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>222</v>
       </c>
@@ -7165,7 +7165,7 @@
       </c>
       <c r="L134" s="5"/>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>222</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>222</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>222</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>222</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="139" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>222</v>
       </c>
@@ -7330,7 +7330,7 @@
       </c>
       <c r="L139" s="5"/>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>222</v>
       </c>
@@ -7353,7 +7353,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="141" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>222</v>
       </c>
@@ -7381,7 +7381,7 @@
       </c>
       <c r="L141" s="5"/>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>270</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>270</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>270</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>270</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>270</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>270</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>270</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>270</v>
       </c>
@@ -7568,7 +7568,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>270</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>270</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>270</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>270</v>
       </c>
@@ -7669,7 +7669,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>270</v>
       </c>
@@ -7692,7 +7692,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>270</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>270</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>270</v>
       </c>
@@ -7770,7 +7770,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>270</v>
       </c>
@@ -7798,7 +7798,7 @@
       </c>
       <c r="L158" s="4"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>270</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>270</v>
       </c>
@@ -7856,7 +7856,7 @@
       </c>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>270</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>270</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>270</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>270</v>
       </c>
@@ -7962,7 +7962,7 @@
       </c>
       <c r="L164" s="4"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>270</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>270</v>
       </c>
@@ -8016,7 +8016,7 @@
       </c>
       <c r="L166" s="4"/>
     </row>
-    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>270</v>
       </c>
@@ -8042,7 +8042,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>270</v>
       </c>
@@ -8072,7 +8072,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>270</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>270</v>
       </c>
@@ -8126,7 +8126,7 @@
       </c>
       <c r="L170" s="4"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>270</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>270</v>
       </c>
@@ -8180,7 +8180,7 @@
       </c>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>270</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>270</v>
       </c>
@@ -8236,7 +8236,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>270</v>
       </c>
@@ -8262,7 +8262,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>270</v>
       </c>
@@ -8290,7 +8290,7 @@
       </c>
       <c r="L176" s="4"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>270</v>
       </c>
@@ -8316,7 +8316,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>364</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
         <v>364</v>
       </c>
@@ -8372,7 +8372,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>64</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>64</v>
       </c>
@@ -8418,7 +8418,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>379</v>
       </c>
@@ -8441,7 +8441,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="183" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>379</v>
       </c>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="L183" s="5"/>
     </row>
-    <row r="184" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>379</v>
       </c>
@@ -8491,7 +8491,7 @@
       <c r="K184" s="5"/>
       <c r="L184" s="5"/>
     </row>
-    <row r="185" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>379</v>
       </c>
@@ -8513,7 +8513,7 @@
       <c r="K185" s="5"/>
       <c r="L185" s="5"/>
     </row>
-    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
         <v>8</v>
       </c>
@@ -8549,7 +8549,7 @@
       </c>
       <c r="L186" s="4"/>
     </row>
-    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>183</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="189" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>183</v>
       </c>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="L189" s="5"/>
     </row>
-    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>183</v>
       </c>
@@ -8658,7 +8658,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="191" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>183</v>
       </c>
@@ -8681,7 +8681,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>183</v>
       </c>
@@ -8704,7 +8704,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="193" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>183</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>183</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="195" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>183</v>
       </c>
@@ -8778,7 +8778,7 @@
       </c>
       <c r="L195" s="5"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>183</v>
       </c>
@@ -8801,7 +8801,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="197" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>183</v>
       </c>
@@ -8829,7 +8829,7 @@
       </c>
       <c r="L197" s="5"/>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>183</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="199" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>183</v>
       </c>
@@ -8880,7 +8880,7 @@
       </c>
       <c r="L199" s="5"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
         <v>422</v>
       </c>
@@ -8908,7 +8908,7 @@
       </c>
       <c r="L200" s="4"/>
     </row>
-    <row r="201" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>422</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
         <v>422</v>
       </c>
@@ -8959,7 +8959,7 @@
       </c>
       <c r="L202" s="4"/>
     </row>
-    <row r="203" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>422</v>
       </c>
@@ -8982,7 +8982,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="204" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>422</v>
       </c>
@@ -9020,7 +9020,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="205" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>422</v>
       </c>
@@ -9058,7 +9058,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="206" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>422</v>
       </c>
@@ -9096,7 +9096,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="207" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>422</v>
       </c>
@@ -9134,7 +9134,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="208" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>422</v>
       </c>
@@ -9172,7 +9172,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="209" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>422</v>
       </c>
@@ -9210,7 +9210,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="210" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>422</v>
       </c>
@@ -9233,7 +9233,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="211" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>422</v>
       </c>
@@ -9256,7 +9256,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="212" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>422</v>
       </c>
@@ -9279,7 +9279,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="213" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>422</v>
       </c>
@@ -9302,7 +9302,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="214" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>422</v>
       </c>
@@ -9325,7 +9325,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="215" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>422</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="216" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>422</v>
       </c>
@@ -9401,7 +9401,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="217" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>422</v>
       </c>
@@ -9439,7 +9439,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="218" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>422</v>
       </c>
@@ -9477,7 +9477,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="219" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>422</v>
       </c>
@@ -9515,7 +9515,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="220" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>422</v>
       </c>
@@ -9553,7 +9553,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>8</v>
       </c>
@@ -9588,7 +9588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>8</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>364</v>
       </c>
@@ -9648,10 +9648,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L223" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
-    <filterColumn colId="10">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Health Prevalency by TPA"/>
-        <filter val="Health Prevalency Percentage"/>
+        <filter val="Mast"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -9669,19 +9668,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="32.26953125" customWidth="1"/>
-    <col min="6" max="6" width="33.453125" customWidth="1"/>
-    <col min="7" max="7" width="31.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9707,12 +9706,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>581</v>
       </c>

</xml_diff>

<commit_message>
added species prevalence for level function
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-Toolbox\fmgpy\summaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CEAFD9-CEC6-4E08-BDBE-15B7399A8AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A116BF04-FE13-43B7-889E-57A1FD0D0B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
+    <workbookView xWindow="40230" yWindow="2330" windowWidth="36220" windowHeight="18850" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="One To One" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="632">
   <si>
     <t>Statistic Category</t>
   </si>
@@ -2232,6 +2232,21 @@
   </si>
   <si>
     <t>02_age_summary</t>
+  </si>
+  <si>
+    <t>tree_table['TR_SP'] == Overstory Sp 1</t>
+  </si>
+  <si>
+    <t>tree_table['TR_SP'] == Overstory Sp 2</t>
+  </si>
+  <si>
+    <t>tree_table['TR_SP'] == Overstory Sp 3</t>
+  </si>
+  <si>
+    <t>tree_table['TR_SP'] == Overstory Sp 4</t>
+  </si>
+  <si>
+    <t>tree_table['TR_SP'] == Overstory Sp 5</t>
   </si>
 </sst>
 </file>
@@ -2848,29 +2863,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D191" sqref="D191"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D174" sqref="D174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" customWidth="1"/>
+    <col min="3" max="3" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="51.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.42578125" customWidth="1"/>
-    <col min="9" max="9" width="59.85546875" customWidth="1"/>
-    <col min="10" max="10" width="53.140625" customWidth="1"/>
-    <col min="11" max="11" width="32.5703125" customWidth="1"/>
-    <col min="12" max="12" width="91.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.453125" customWidth="1"/>
+    <col min="9" max="9" width="59.81640625" customWidth="1"/>
+    <col min="10" max="10" width="53.1796875" customWidth="1"/>
+    <col min="11" max="11" width="32.54296875" customWidth="1"/>
+    <col min="12" max="12" width="91.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2908,7 +2924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2940,7 +2956,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2972,7 +2988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -3006,7 +3022,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3041,7 +3057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -3077,7 +3093,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3112,7 +3128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3138,7 +3154,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3173,7 +3189,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -3209,7 +3225,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -3245,7 +3261,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3280,7 +3296,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3315,7 +3331,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3347,7 +3363,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -3381,7 +3397,7 @@
       </c>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -3415,7 +3431,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -3449,7 +3465,7 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3481,7 +3497,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
@@ -3515,7 +3531,7 @@
       </c>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
@@ -3551,7 +3567,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3586,7 +3602,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -3620,7 +3636,7 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3652,7 +3668,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3684,7 +3700,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3716,7 +3732,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -3748,7 +3764,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>64</v>
       </c>
@@ -3784,7 +3800,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3822,7 +3838,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3860,7 +3876,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -3898,7 +3914,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -3936,7 +3952,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
@@ -3972,7 +3988,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>85</v>
       </c>
@@ -4010,7 +4026,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -4048,7 +4064,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -4086,7 +4102,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -4121,7 +4137,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>85</v>
       </c>
@@ -4157,7 +4173,7 @@
       </c>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
@@ -4185,7 +4201,7 @@
       </c>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>85</v>
       </c>
@@ -4213,7 +4229,7 @@
       </c>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -4251,7 +4267,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -4289,7 +4305,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -4327,7 +4343,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -4365,7 +4381,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>85</v>
       </c>
@@ -4403,7 +4419,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -4441,7 +4457,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>85</v>
       </c>
@@ -4477,7 +4493,7 @@
       </c>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>85</v>
       </c>
@@ -4513,7 +4529,7 @@
       </c>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -4536,7 +4552,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -4564,7 +4580,7 @@
       </c>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -4602,7 +4618,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>85</v>
       </c>
@@ -4640,7 +4656,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -4678,7 +4694,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>85</v>
       </c>
@@ -4716,7 +4732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -4754,7 +4770,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -4792,7 +4808,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -4827,7 +4843,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>85</v>
       </c>
@@ -4863,7 +4879,7 @@
       </c>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>85</v>
       </c>
@@ -4891,7 +4907,7 @@
       </c>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>85</v>
       </c>
@@ -4919,7 +4935,7 @@
       </c>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>85</v>
       </c>
@@ -4957,7 +4973,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -4995,7 +5011,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -5033,7 +5049,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -5071,7 +5087,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -5109,7 +5125,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>85</v>
       </c>
@@ -5147,7 +5163,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -5182,7 +5198,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>85</v>
       </c>
@@ -5217,7 +5233,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -5240,7 +5256,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>85</v>
       </c>
@@ -5268,7 +5284,7 @@
       </c>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -5306,7 +5322,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -5344,7 +5360,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -5382,7 +5398,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -5420,7 +5436,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -5458,7 +5474,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -5496,7 +5512,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -5531,7 +5547,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="77" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>85</v>
       </c>
@@ -5567,7 +5583,7 @@
       </c>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -5590,7 +5606,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>85</v>
       </c>
@@ -5618,7 +5634,7 @@
       </c>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -5656,7 +5672,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -5694,7 +5710,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -5732,7 +5748,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>85</v>
       </c>
@@ -5770,7 +5786,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>85</v>
       </c>
@@ -5808,7 +5824,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>85</v>
       </c>
@@ -5846,7 +5862,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>85</v>
       </c>
@@ -5882,7 +5898,7 @@
       </c>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>85</v>
       </c>
@@ -5918,7 +5934,7 @@
       </c>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>85</v>
       </c>
@@ -5946,7 +5962,7 @@
       </c>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>85</v>
       </c>
@@ -5974,7 +5990,7 @@
       </c>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>85</v>
       </c>
@@ -6012,7 +6028,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>85</v>
       </c>
@@ -6050,7 +6066,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>85</v>
       </c>
@@ -6088,7 +6104,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>183</v>
       </c>
@@ -6126,7 +6142,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -6164,7 +6180,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>183</v>
       </c>
@@ -6202,7 +6218,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>183</v>
       </c>
@@ -6225,7 +6241,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="97" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>183</v>
       </c>
@@ -6248,7 +6264,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>183</v>
       </c>
@@ -6286,7 +6302,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>183</v>
       </c>
@@ -6324,7 +6340,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>183</v>
       </c>
@@ -6362,7 +6378,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>183</v>
       </c>
@@ -6385,7 +6401,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="102" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>183</v>
       </c>
@@ -6413,7 +6429,7 @@
       </c>
       <c r="L102" s="5"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>183</v>
       </c>
@@ -6451,7 +6467,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>183</v>
       </c>
@@ -6489,7 +6505,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>183</v>
       </c>
@@ -6527,7 +6543,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>183</v>
       </c>
@@ -6550,7 +6566,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="107" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>183</v>
       </c>
@@ -6573,7 +6589,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>183</v>
       </c>
@@ -6611,7 +6627,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>183</v>
       </c>
@@ -6649,7 +6665,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>183</v>
       </c>
@@ -6687,7 +6703,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>183</v>
       </c>
@@ -6710,7 +6726,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="112" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>183</v>
       </c>
@@ -6738,7 +6754,7 @@
       </c>
       <c r="L112" s="5"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>183</v>
       </c>
@@ -6764,7 +6780,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>222</v>
       </c>
@@ -6802,7 +6818,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>222</v>
       </c>
@@ -6840,7 +6856,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>222</v>
       </c>
@@ -6878,7 +6894,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>222</v>
       </c>
@@ -6913,7 +6929,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="118" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>222</v>
       </c>
@@ -6948,7 +6964,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>222</v>
       </c>
@@ -6976,7 +6992,7 @@
       </c>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>222</v>
       </c>
@@ -6999,7 +7015,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>222</v>
       </c>
@@ -7037,7 +7053,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>222</v>
       </c>
@@ -7075,7 +7091,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>222</v>
       </c>
@@ -7113,7 +7129,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>222</v>
       </c>
@@ -7149,7 +7165,7 @@
       </c>
       <c r="L124" s="4"/>
     </row>
-    <row r="125" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>222</v>
       </c>
@@ -7184,7 +7200,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>222</v>
       </c>
@@ -7212,7 +7228,7 @@
       </c>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>222</v>
       </c>
@@ -7235,7 +7251,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>222</v>
       </c>
@@ -7273,7 +7289,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>222</v>
       </c>
@@ -7311,7 +7327,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>222</v>
       </c>
@@ -7349,7 +7365,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>222</v>
       </c>
@@ -7384,7 +7400,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="132" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>222</v>
       </c>
@@ -7419,7 +7435,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>222</v>
       </c>
@@ -7442,7 +7458,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="134" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>222</v>
       </c>
@@ -7470,7 +7486,7 @@
       </c>
       <c r="L134" s="5"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>222</v>
       </c>
@@ -7508,7 +7524,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>222</v>
       </c>
@@ -7546,7 +7562,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>222</v>
       </c>
@@ -7584,7 +7600,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>222</v>
       </c>
@@ -7619,7 +7635,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="139" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>222</v>
       </c>
@@ -7655,7 +7671,7 @@
       </c>
       <c r="L139" s="5"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>222</v>
       </c>
@@ -7678,7 +7694,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="141" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>222</v>
       </c>
@@ -7706,7 +7722,7 @@
       </c>
       <c r="L141" s="5"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>270</v>
       </c>
@@ -7729,7 +7745,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>270</v>
       </c>
@@ -7752,7 +7768,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>270</v>
       </c>
@@ -7775,7 +7791,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>270</v>
       </c>
@@ -7798,7 +7814,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>270</v>
       </c>
@@ -7821,7 +7837,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>270</v>
       </c>
@@ -7844,7 +7860,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>270</v>
       </c>
@@ -7867,10 +7883,22 @@
         <v>288</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>270</v>
       </c>
+      <c r="B149" t="s">
+        <v>584</v>
+      </c>
+      <c r="C149" t="s">
+        <v>592</v>
+      </c>
+      <c r="D149" t="s">
+        <v>627</v>
+      </c>
+      <c r="E149" t="s">
+        <v>594</v>
+      </c>
       <c r="F149" t="s">
         <v>289</v>
       </c>
@@ -7893,10 +7921,22 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>270</v>
       </c>
+      <c r="B150" t="s">
+        <v>584</v>
+      </c>
+      <c r="C150" t="s">
+        <v>592</v>
+      </c>
+      <c r="D150" t="s">
+        <v>627</v>
+      </c>
+      <c r="E150" t="s">
+        <v>594</v>
+      </c>
       <c r="F150" t="s">
         <v>292</v>
       </c>
@@ -7919,10 +7959,22 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>270</v>
       </c>
+      <c r="B151" t="s">
+        <v>584</v>
+      </c>
+      <c r="C151" t="s">
+        <v>592</v>
+      </c>
+      <c r="D151" t="s">
+        <v>627</v>
+      </c>
+      <c r="E151" t="s">
+        <v>594</v>
+      </c>
       <c r="F151" t="s">
         <v>294</v>
       </c>
@@ -7945,10 +7997,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>270</v>
       </c>
+      <c r="B152" t="s">
+        <v>584</v>
+      </c>
+      <c r="C152" t="s">
+        <v>603</v>
+      </c>
+      <c r="D152" t="s">
+        <v>627</v>
+      </c>
+      <c r="E152" t="s">
+        <v>594</v>
+      </c>
       <c r="F152" t="s">
         <v>296</v>
       </c>
@@ -7968,10 +8032,22 @@
         <v>599</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>270</v>
       </c>
+      <c r="B153" t="s">
+        <v>584</v>
+      </c>
+      <c r="C153" t="s">
+        <v>603</v>
+      </c>
+      <c r="D153" t="s">
+        <v>627</v>
+      </c>
+      <c r="E153" t="s">
+        <v>594</v>
+      </c>
       <c r="F153" t="s">
         <v>299</v>
       </c>
@@ -7994,7 +8070,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>270</v>
       </c>
@@ -8017,10 +8093,22 @@
         <v>288</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>270</v>
       </c>
+      <c r="B155" t="s">
+        <v>584</v>
+      </c>
+      <c r="C155" t="s">
+        <v>592</v>
+      </c>
+      <c r="D155" t="s">
+        <v>628</v>
+      </c>
+      <c r="E155" t="s">
+        <v>594</v>
+      </c>
       <c r="F155" t="s">
         <v>306</v>
       </c>
@@ -8043,10 +8131,22 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>270</v>
       </c>
+      <c r="B156" t="s">
+        <v>584</v>
+      </c>
+      <c r="C156" t="s">
+        <v>592</v>
+      </c>
+      <c r="D156" t="s">
+        <v>628</v>
+      </c>
+      <c r="E156" t="s">
+        <v>594</v>
+      </c>
       <c r="F156" t="s">
         <v>309</v>
       </c>
@@ -8069,10 +8169,22 @@
         <v>74</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>270</v>
       </c>
+      <c r="B157" t="s">
+        <v>584</v>
+      </c>
+      <c r="C157" t="s">
+        <v>592</v>
+      </c>
+      <c r="D157" t="s">
+        <v>628</v>
+      </c>
+      <c r="E157" t="s">
+        <v>594</v>
+      </c>
       <c r="F157" t="s">
         <v>311</v>
       </c>
@@ -8095,14 +8207,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B158" s="4"/>
-      <c r="C158" s="4"/>
-      <c r="D158" s="4"/>
-      <c r="E158" s="4"/>
+      <c r="B158" t="s">
+        <v>584</v>
+      </c>
+      <c r="C158" t="s">
+        <v>603</v>
+      </c>
+      <c r="D158" t="s">
+        <v>628</v>
+      </c>
+      <c r="E158" t="s">
+        <v>594</v>
+      </c>
       <c r="F158" s="4" t="s">
         <v>313</v>
       </c>
@@ -8123,14 +8243,22 @@
       </c>
       <c r="L158" s="4"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B159" s="4"/>
-      <c r="C159" s="4"/>
-      <c r="D159" s="4"/>
-      <c r="E159" s="4"/>
+      <c r="B159" t="s">
+        <v>584</v>
+      </c>
+      <c r="C159" t="s">
+        <v>603</v>
+      </c>
+      <c r="D159" t="s">
+        <v>628</v>
+      </c>
+      <c r="E159" t="s">
+        <v>594</v>
+      </c>
       <c r="F159" s="4" t="s">
         <v>316</v>
       </c>
@@ -8153,7 +8281,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>270</v>
       </c>
@@ -8181,10 +8309,22 @@
       </c>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>270</v>
       </c>
+      <c r="B161" t="s">
+        <v>584</v>
+      </c>
+      <c r="C161" t="s">
+        <v>592</v>
+      </c>
+      <c r="D161" t="s">
+        <v>629</v>
+      </c>
+      <c r="E161" t="s">
+        <v>594</v>
+      </c>
       <c r="F161" t="s">
         <v>322</v>
       </c>
@@ -8207,10 +8347,22 @@
         <v>79</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>270</v>
       </c>
+      <c r="B162" t="s">
+        <v>584</v>
+      </c>
+      <c r="C162" t="s">
+        <v>592</v>
+      </c>
+      <c r="D162" t="s">
+        <v>629</v>
+      </c>
+      <c r="E162" t="s">
+        <v>594</v>
+      </c>
       <c r="F162" t="s">
         <v>325</v>
       </c>
@@ -8233,10 +8385,22 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>270</v>
       </c>
+      <c r="B163" t="s">
+        <v>584</v>
+      </c>
+      <c r="C163" t="s">
+        <v>592</v>
+      </c>
+      <c r="D163" t="s">
+        <v>629</v>
+      </c>
+      <c r="E163" t="s">
+        <v>594</v>
+      </c>
       <c r="F163" t="s">
         <v>327</v>
       </c>
@@ -8259,14 +8423,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B164" s="4"/>
-      <c r="C164" s="4"/>
-      <c r="D164" s="4"/>
-      <c r="E164" s="4"/>
+      <c r="B164" t="s">
+        <v>584</v>
+      </c>
+      <c r="C164" t="s">
+        <v>603</v>
+      </c>
+      <c r="D164" t="s">
+        <v>629</v>
+      </c>
+      <c r="E164" t="s">
+        <v>594</v>
+      </c>
       <c r="F164" s="4" t="s">
         <v>329</v>
       </c>
@@ -8287,10 +8459,22 @@
       </c>
       <c r="L164" s="4"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>270</v>
       </c>
+      <c r="B165" t="s">
+        <v>584</v>
+      </c>
+      <c r="C165" t="s">
+        <v>603</v>
+      </c>
+      <c r="D165" t="s">
+        <v>629</v>
+      </c>
+      <c r="E165" t="s">
+        <v>594</v>
+      </c>
       <c r="F165" t="s">
         <v>332</v>
       </c>
@@ -8313,7 +8497,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
         <v>270</v>
       </c>
@@ -8341,10 +8525,22 @@
       </c>
       <c r="L166" s="4"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>270</v>
       </c>
+      <c r="B167" t="s">
+        <v>584</v>
+      </c>
+      <c r="C167" t="s">
+        <v>592</v>
+      </c>
+      <c r="D167" t="s">
+        <v>630</v>
+      </c>
+      <c r="E167" t="s">
+        <v>594</v>
+      </c>
       <c r="F167" t="s">
         <v>337</v>
       </c>
@@ -8367,14 +8563,22 @@
         <v>79</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B168" s="4"/>
-      <c r="C168" s="4"/>
-      <c r="D168" s="4"/>
-      <c r="E168" s="4"/>
+      <c r="B168" t="s">
+        <v>584</v>
+      </c>
+      <c r="C168" t="s">
+        <v>592</v>
+      </c>
+      <c r="D168" t="s">
+        <v>630</v>
+      </c>
+      <c r="E168" t="s">
+        <v>594</v>
+      </c>
       <c r="F168" s="4" t="s">
         <v>340</v>
       </c>
@@ -8397,10 +8601,22 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>270</v>
       </c>
+      <c r="B169" t="s">
+        <v>584</v>
+      </c>
+      <c r="C169" t="s">
+        <v>592</v>
+      </c>
+      <c r="D169" t="s">
+        <v>630</v>
+      </c>
+      <c r="E169" t="s">
+        <v>594</v>
+      </c>
       <c r="F169" t="s">
         <v>342</v>
       </c>
@@ -8423,14 +8639,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B170" s="4"/>
-      <c r="C170" s="4"/>
-      <c r="D170" s="4"/>
-      <c r="E170" s="4"/>
+      <c r="B170" t="s">
+        <v>584</v>
+      </c>
+      <c r="C170" t="s">
+        <v>603</v>
+      </c>
+      <c r="D170" t="s">
+        <v>630</v>
+      </c>
+      <c r="E170" t="s">
+        <v>594</v>
+      </c>
       <c r="F170" s="4" t="s">
         <v>344</v>
       </c>
@@ -8451,10 +8675,22 @@
       </c>
       <c r="L170" s="4"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>270</v>
       </c>
+      <c r="B171" t="s">
+        <v>584</v>
+      </c>
+      <c r="C171" t="s">
+        <v>603</v>
+      </c>
+      <c r="D171" t="s">
+        <v>630</v>
+      </c>
+      <c r="E171" t="s">
+        <v>594</v>
+      </c>
       <c r="F171" t="s">
         <v>347</v>
       </c>
@@ -8477,7 +8713,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
         <v>270</v>
       </c>
@@ -8505,10 +8741,22 @@
       </c>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>270</v>
       </c>
+      <c r="B173" t="s">
+        <v>584</v>
+      </c>
+      <c r="C173" t="s">
+        <v>592</v>
+      </c>
+      <c r="D173" t="s">
+        <v>631</v>
+      </c>
+      <c r="E173" t="s">
+        <v>594</v>
+      </c>
       <c r="F173" t="s">
         <v>352</v>
       </c>
@@ -8531,14 +8779,22 @@
         <v>79</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B174" s="4"/>
-      <c r="C174" s="4"/>
-      <c r="D174" s="4"/>
-      <c r="E174" s="4"/>
+      <c r="B174" t="s">
+        <v>584</v>
+      </c>
+      <c r="C174" t="s">
+        <v>592</v>
+      </c>
+      <c r="D174" t="s">
+        <v>631</v>
+      </c>
+      <c r="E174" t="s">
+        <v>594</v>
+      </c>
       <c r="F174" s="4" t="s">
         <v>355</v>
       </c>
@@ -8561,10 +8817,22 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>270</v>
       </c>
+      <c r="B175" t="s">
+        <v>584</v>
+      </c>
+      <c r="C175" t="s">
+        <v>592</v>
+      </c>
+      <c r="D175" t="s">
+        <v>631</v>
+      </c>
+      <c r="E175" t="s">
+        <v>594</v>
+      </c>
       <c r="F175" t="s">
         <v>357</v>
       </c>
@@ -8587,14 +8855,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B176" s="4"/>
-      <c r="C176" s="4"/>
-      <c r="D176" s="4"/>
-      <c r="E176" s="4"/>
+      <c r="B176" t="s">
+        <v>584</v>
+      </c>
+      <c r="C176" t="s">
+        <v>603</v>
+      </c>
+      <c r="D176" t="s">
+        <v>631</v>
+      </c>
+      <c r="E176" t="s">
+        <v>594</v>
+      </c>
       <c r="F176" s="4" t="s">
         <v>359</v>
       </c>
@@ -8615,10 +8891,22 @@
       </c>
       <c r="L176" s="4"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>270</v>
       </c>
+      <c r="B177" t="s">
+        <v>584</v>
+      </c>
+      <c r="C177" t="s">
+        <v>603</v>
+      </c>
+      <c r="D177" t="s">
+        <v>631</v>
+      </c>
+      <c r="E177" t="s">
+        <v>594</v>
+      </c>
       <c r="F177" t="s">
         <v>362</v>
       </c>
@@ -8641,7 +8929,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>364</v>
       </c>
@@ -8667,7 +8955,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
         <v>364</v>
       </c>
@@ -8697,7 +8985,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>64</v>
       </c>
@@ -8732,7 +9020,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>64</v>
       </c>
@@ -8767,7 +9055,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>379</v>
       </c>
@@ -8790,7 +9078,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="183" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>379</v>
       </c>
@@ -8816,7 +9104,7 @@
       </c>
       <c r="L183" s="5"/>
     </row>
-    <row r="184" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
         <v>379</v>
       </c>
@@ -8840,7 +9128,7 @@
       <c r="K184" s="5"/>
       <c r="L184" s="5"/>
     </row>
-    <row r="185" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>379</v>
       </c>
@@ -8862,7 +9150,7 @@
       <c r="K185" s="5"/>
       <c r="L185" s="5"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="4" t="s">
         <v>8</v>
       </c>
@@ -8898,7 +9186,7 @@
       </c>
       <c r="L186" s="4"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -8933,7 +9221,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>183</v>
       </c>
@@ -8968,7 +9256,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="189" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
         <v>183</v>
       </c>
@@ -9004,7 +9292,7 @@
       </c>
       <c r="L189" s="5"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>183</v>
       </c>
@@ -9027,7 +9315,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="191" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
         <v>183</v>
       </c>
@@ -9050,7 +9338,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>183</v>
       </c>
@@ -9085,7 +9373,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="193" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
         <v>183</v>
       </c>
@@ -9120,7 +9408,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>183</v>
       </c>
@@ -9143,7 +9431,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="195" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>183</v>
       </c>
@@ -9171,7 +9459,7 @@
       </c>
       <c r="L195" s="5"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>183</v>
       </c>
@@ -9206,7 +9494,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="197" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
         <v>183</v>
       </c>
@@ -9242,7 +9530,7 @@
       </c>
       <c r="L197" s="5"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>183</v>
       </c>
@@ -9265,7 +9553,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="199" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>183</v>
       </c>
@@ -9293,7 +9581,7 @@
       </c>
       <c r="L199" s="5"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" s="4" t="s">
         <v>422</v>
       </c>
@@ -9329,7 +9617,7 @@
       </c>
       <c r="L200" s="4"/>
     </row>
-    <row r="201" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
         <v>422</v>
       </c>
@@ -9364,7 +9652,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="4" t="s">
         <v>422</v>
       </c>
@@ -9392,7 +9680,7 @@
       </c>
       <c r="L202" s="4"/>
     </row>
-    <row r="203" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
         <v>422</v>
       </c>
@@ -9415,7 +9703,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="204" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
         <v>422</v>
       </c>
@@ -9453,7 +9741,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="205" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
         <v>422</v>
       </c>
@@ -9491,7 +9779,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="206" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
         <v>422</v>
       </c>
@@ -9529,7 +9817,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="207" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
         <v>422</v>
       </c>
@@ -9567,7 +9855,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="208" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" s="2" t="s">
         <v>422</v>
       </c>
@@ -9605,7 +9893,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="209" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" s="2" t="s">
         <v>422</v>
       </c>
@@ -9643,7 +9931,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="210" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" s="2" t="s">
         <v>422</v>
       </c>
@@ -9678,7 +9966,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="211" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
         <v>422</v>
       </c>
@@ -9713,7 +10001,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="212" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
         <v>422</v>
       </c>
@@ -9736,7 +10024,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="213" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
         <v>422</v>
       </c>
@@ -9759,7 +10047,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="214" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
         <v>422</v>
       </c>
@@ -9794,7 +10082,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="215" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
         <v>422</v>
       </c>
@@ -9829,7 +10117,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="216" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>422</v>
       </c>
@@ -9852,7 +10140,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="217" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>422</v>
       </c>
@@ -9875,7 +10163,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="218" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" s="2" t="s">
         <v>422</v>
       </c>
@@ -9913,7 +10201,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="219" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" s="2" t="s">
         <v>422</v>
       </c>
@@ -9951,7 +10239,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="220" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" s="2" t="s">
         <v>422</v>
       </c>
@@ -9989,7 +10277,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="221" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" s="5" t="s">
         <v>422</v>
       </c>
@@ -10027,7 +10315,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="222" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
         <v>422</v>
       </c>
@@ -10065,7 +10353,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="223" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" s="5" t="s">
         <v>422</v>
       </c>
@@ -10103,7 +10391,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>8</v>
       </c>
@@ -10138,7 +10426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>8</v>
       </c>
@@ -10173,7 +10461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>364</v>
       </c>
@@ -10197,7 +10485,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L226" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}"/>
+  <autoFilter ref="A1:L226" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="Species Prevalency by TPA"/>
+        <filter val="Species Prevalency Percentage"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -10212,19 +10507,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="32.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.453125" customWidth="1"/>
+    <col min="7" max="7" width="31.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10250,12 +10545,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>579</v>
       </c>

</xml_diff>

<commit_message>
added species prevalence plot function
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A116BF04-FE13-43B7-889E-57A1FD0D0B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74929529-CDF4-4869-95ED-A7D3EBB2B126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40230" yWindow="2330" windowWidth="36220" windowHeight="18850" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
+    <workbookView xWindow="39980" yWindow="1460" windowWidth="36220" windowHeight="18850" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="One To One" sheetId="1" r:id="rId1"/>
@@ -2867,7 +2867,7 @@
   <dimension ref="A1:L226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D174" sqref="D174"/>
+      <selection activeCell="F244" sqref="F244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2924,7 +2924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
@@ -3567,7 +3567,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>85</v>
       </c>
@@ -4529,7 +4529,7 @@
       </c>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -4879,7 +4879,7 @@
       </c>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>85</v>
       </c>
@@ -4907,7 +4907,7 @@
       </c>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>85</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>85</v>
       </c>
@@ -5583,7 +5583,7 @@
       </c>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>85</v>
       </c>
@@ -5934,7 +5934,7 @@
       </c>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>85</v>
       </c>
@@ -5962,7 +5962,7 @@
       </c>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>85</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>183</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="97" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>183</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>183</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="102" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>183</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>183</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="107" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>183</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>183</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="112" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>183</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>222</v>
       </c>
@@ -6992,7 +6992,7 @@
       </c>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>222</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>222</v>
       </c>
@@ -7228,7 +7228,7 @@
       </c>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>222</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>222</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="134" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>222</v>
       </c>
@@ -7671,7 +7671,7 @@
       </c>
       <c r="L139" s="5"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>222</v>
       </c>
@@ -7694,7 +7694,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="141" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>222</v>
       </c>
@@ -9150,7 +9150,7 @@
       <c r="K185" s="5"/>
       <c r="L185" s="5"/>
     </row>
-    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A186" s="4" t="s">
         <v>8</v>
       </c>
@@ -9186,7 +9186,7 @@
       </c>
       <c r="L186" s="4"/>
     </row>
-    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -9292,7 +9292,7 @@
       </c>
       <c r="L189" s="5"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>183</v>
       </c>
@@ -9315,7 +9315,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="191" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
         <v>183</v>
       </c>
@@ -9408,7 +9408,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>183</v>
       </c>
@@ -9431,7 +9431,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="195" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>183</v>
       </c>
@@ -9530,7 +9530,7 @@
       </c>
       <c r="L197" s="5"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>183</v>
       </c>
@@ -9553,7 +9553,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="199" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>183</v>
       </c>
@@ -9652,7 +9652,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" s="4" t="s">
         <v>422</v>
       </c>
@@ -9680,7 +9680,7 @@
       </c>
       <c r="L202" s="4"/>
     </row>
-    <row r="203" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
         <v>422</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="212" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
         <v>422</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="213" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
         <v>422</v>
       </c>
@@ -10117,7 +10117,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="216" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>422</v>
       </c>
@@ -10140,7 +10140,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="217" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>422</v>
       </c>
@@ -10391,7 +10391,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>8</v>
       </c>
@@ -10426,7 +10426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>8</v>
       </c>
@@ -10486,10 +10486,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L226" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
-    <filterColumn colId="10">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Species Prevalency by TPA"/>
-        <filter val="Species Prevalency Percentage"/>
+        <filter val="General Descriptive"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
wrote overstory sp pattern
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74929529-CDF4-4869-95ED-A7D3EBB2B126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2371CF-FDC3-4EB3-9949-0BEFC85738BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39980" yWindow="1460" windowWidth="36220" windowHeight="18850" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
+    <workbookView xWindow="39980" yWindow="470" windowWidth="36220" windowHeight="18850" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="One To One" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="638">
   <si>
     <t>Statistic Category</t>
   </si>
@@ -2247,6 +2247,24 @@
   </si>
   <si>
     <t>tree_table['TR_SP'] == Overstory Sp 5</t>
+  </si>
+  <si>
+    <t>forest_calcs.species_prev_pct_level &amp; plot</t>
+  </si>
+  <si>
+    <t>TR_SP</t>
+  </si>
+  <si>
+    <t>tree_table['TR_HLTH'] == 'D'</t>
+  </si>
+  <si>
+    <t>tree_table['TR_HLTH'] == 'SD'</t>
+  </si>
+  <si>
+    <t>tree_table['TR_HLTH'] == 'S'</t>
+  </si>
+  <si>
+    <t>tree_table['TR_HLTH'] == 'H'</t>
   </si>
 </sst>
 </file>
@@ -2863,11 +2881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F244" sqref="F244"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3636,7 +3653,7 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -3668,7 +3685,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3700,7 +3717,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3732,7 +3749,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -3764,7 +3781,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>64</v>
       </c>
@@ -3988,7 +4005,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>85</v>
       </c>
@@ -4026,7 +4043,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -4064,7 +4081,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -4102,7 +4119,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -4137,7 +4154,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>85</v>
       </c>
@@ -4173,14 +4190,22 @@
       </c>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="B38" t="s">
+        <v>584</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D38" t="s">
+        <v>604</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F38" s="4" t="s">
         <v>97</v>
       </c>
@@ -4201,14 +4226,22 @@
       </c>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="B39" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F39" s="5" t="s">
         <v>482</v>
       </c>
@@ -4229,7 +4262,7 @@
       </c>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -4267,7 +4300,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -4305,7 +4338,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -4343,7 +4376,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -4381,7 +4414,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>85</v>
       </c>
@@ -4419,7 +4452,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -4457,7 +4490,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>85</v>
       </c>
@@ -4493,7 +4526,7 @@
       </c>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>85</v>
       </c>
@@ -4529,10 +4562,22 @@
       </c>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>85</v>
       </c>
+      <c r="B48" t="s">
+        <v>584</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F48" t="s">
         <v>117</v>
       </c>
@@ -4552,14 +4597,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="B49" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F49" s="5" t="s">
         <v>491</v>
       </c>
@@ -4580,7 +4633,7 @@
       </c>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -4618,7 +4671,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>85</v>
       </c>
@@ -4656,7 +4709,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -4694,7 +4747,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>85</v>
       </c>
@@ -4732,7 +4785,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -4770,7 +4823,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -4808,7 +4861,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -4843,7 +4896,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>85</v>
       </c>
@@ -4879,14 +4932,22 @@
       </c>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
+      <c r="B58" t="s">
+        <v>584</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D58" t="s">
+        <v>606</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F58" s="4" t="s">
         <v>136</v>
       </c>
@@ -4907,14 +4968,22 @@
       </c>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
+      <c r="B59" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F59" s="5" t="s">
         <v>495</v>
       </c>
@@ -4935,7 +5004,7 @@
       </c>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>85</v>
       </c>
@@ -4973,7 +5042,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -5011,7 +5080,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -5049,7 +5118,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -5087,7 +5156,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -5125,7 +5194,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>85</v>
       </c>
@@ -5163,7 +5232,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -5198,7 +5267,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>85</v>
       </c>
@@ -5233,10 +5302,22 @@
         <v>600</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>85</v>
       </c>
+      <c r="B68" t="s">
+        <v>584</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D68" t="s">
+        <v>607</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F68" t="s">
         <v>155</v>
       </c>
@@ -5256,14 +5337,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
+      <c r="B69" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F69" s="5" t="s">
         <v>499</v>
       </c>
@@ -5284,7 +5373,7 @@
       </c>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -5322,7 +5411,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -5360,7 +5449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -5398,7 +5487,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -5436,7 +5525,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -5474,7 +5563,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -5512,7 +5601,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -5547,7 +5636,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="77" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>85</v>
       </c>
@@ -5583,10 +5672,22 @@
       </c>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>85</v>
       </c>
+      <c r="B78" t="s">
+        <v>584</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D78" t="s">
+        <v>608</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F78" t="s">
         <v>174</v>
       </c>
@@ -5606,14 +5707,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
+      <c r="B79" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F79" s="5" t="s">
         <v>503</v>
       </c>
@@ -5634,7 +5743,7 @@
       </c>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -5672,7 +5781,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -5710,7 +5819,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -5748,7 +5857,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>85</v>
       </c>
@@ -5786,7 +5895,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>85</v>
       </c>
@@ -5824,7 +5933,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>85</v>
       </c>
@@ -5862,7 +5971,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>85</v>
       </c>
@@ -5898,7 +6007,7 @@
       </c>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>85</v>
       </c>
@@ -5934,14 +6043,22 @@
       </c>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
+      <c r="B88" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F88" s="5" t="s">
         <v>515</v>
       </c>
@@ -5962,14 +6079,22 @@
       </c>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
+      <c r="B89" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F89" s="5" t="s">
         <v>516</v>
       </c>
@@ -5990,7 +6115,7 @@
       </c>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>85</v>
       </c>
@@ -6028,7 +6153,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>85</v>
       </c>
@@ -6066,7 +6191,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>85</v>
       </c>
@@ -6104,7 +6229,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>183</v>
       </c>
@@ -6142,7 +6267,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -6180,7 +6305,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>183</v>
       </c>
@@ -6218,10 +6343,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>183</v>
       </c>
+      <c r="B96" t="s">
+        <v>584</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D96" t="s">
+        <v>634</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F96" t="s">
         <v>190</v>
       </c>
@@ -6241,10 +6378,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="97" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>183</v>
       </c>
+      <c r="B97" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F97" s="2" t="s">
         <v>534</v>
       </c>
@@ -6264,7 +6413,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>183</v>
       </c>
@@ -6302,7 +6451,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>183</v>
       </c>
@@ -6340,7 +6489,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>183</v>
       </c>
@@ -6378,10 +6527,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>183</v>
       </c>
+      <c r="B101" t="s">
+        <v>584</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D101" t="s">
+        <v>635</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F101" t="s">
         <v>199</v>
       </c>
@@ -6401,14 +6562,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="102" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
+      <c r="B102" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F102" s="5" t="s">
         <v>535</v>
       </c>
@@ -6429,7 +6598,7 @@
       </c>
       <c r="L102" s="5"/>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>183</v>
       </c>
@@ -6467,7 +6636,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>183</v>
       </c>
@@ -6505,7 +6674,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>183</v>
       </c>
@@ -6543,10 +6712,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>183</v>
       </c>
+      <c r="B106" t="s">
+        <v>584</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D106" t="s">
+        <v>636</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F106" t="s">
         <v>208</v>
       </c>
@@ -6566,10 +6747,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="107" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>183</v>
       </c>
+      <c r="B107" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F107" s="2" t="s">
         <v>536</v>
       </c>
@@ -6589,7 +6782,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>183</v>
       </c>
@@ -6627,7 +6820,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>183</v>
       </c>
@@ -6665,7 +6858,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>183</v>
       </c>
@@ -6703,10 +6896,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>183</v>
       </c>
+      <c r="B111" t="s">
+        <v>584</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D111" t="s">
+        <v>637</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F111" t="s">
         <v>217</v>
       </c>
@@ -6726,14 +6931,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="112" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
+      <c r="B112" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F112" s="5" t="s">
         <v>537</v>
       </c>
@@ -6754,7 +6967,7 @@
       </c>
       <c r="L112" s="5"/>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>183</v>
       </c>
@@ -6780,7 +6993,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>222</v>
       </c>
@@ -6818,7 +7031,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>222</v>
       </c>
@@ -6856,7 +7069,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>222</v>
       </c>
@@ -6894,7 +7107,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>222</v>
       </c>
@@ -6929,7 +7142,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="118" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>222</v>
       </c>
@@ -6964,14 +7177,22 @@
         <v>600</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
+      <c r="B119" t="s">
+        <v>584</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D119" t="s">
+        <v>610</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F119" s="4" t="s">
         <v>233</v>
       </c>
@@ -6992,10 +7213,22 @@
       </c>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>222</v>
       </c>
+      <c r="B120" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F120" s="2" t="s">
         <v>539</v>
       </c>
@@ -7015,7 +7248,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>222</v>
       </c>
@@ -7053,7 +7286,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>222</v>
       </c>
@@ -7091,7 +7324,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>222</v>
       </c>
@@ -7129,7 +7362,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>222</v>
       </c>
@@ -7165,7 +7398,7 @@
       </c>
       <c r="L124" s="4"/>
     </row>
-    <row r="125" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>222</v>
       </c>
@@ -7200,14 +7433,22 @@
         <v>600</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B126" s="4"/>
-      <c r="C126" s="4"/>
-      <c r="D126" s="4"/>
-      <c r="E126" s="4"/>
+      <c r="B126" t="s">
+        <v>584</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F126" s="4" t="s">
         <v>245</v>
       </c>
@@ -7228,10 +7469,22 @@
       </c>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>222</v>
       </c>
+      <c r="B127" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F127" s="2" t="s">
         <v>541</v>
       </c>
@@ -7251,7 +7504,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>222</v>
       </c>
@@ -7289,7 +7542,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>222</v>
       </c>
@@ -7327,7 +7580,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>222</v>
       </c>
@@ -7365,7 +7618,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>222</v>
       </c>
@@ -7400,7 +7653,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="132" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>222</v>
       </c>
@@ -7435,10 +7688,22 @@
         <v>600</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>222</v>
       </c>
+      <c r="B133" t="s">
+        <v>584</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D133" t="s">
+        <v>612</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F133" t="s">
         <v>256</v>
       </c>
@@ -7458,14 +7723,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="134" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B134" s="5"/>
-      <c r="C134" s="5"/>
-      <c r="D134" s="5"/>
-      <c r="E134" s="5"/>
+      <c r="B134" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F134" s="5" t="s">
         <v>542</v>
       </c>
@@ -7486,7 +7759,7 @@
       </c>
       <c r="L134" s="5"/>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>222</v>
       </c>
@@ -7524,7 +7797,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>222</v>
       </c>
@@ -7562,7 +7835,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>222</v>
       </c>
@@ -7600,7 +7873,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>222</v>
       </c>
@@ -7635,7 +7908,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="139" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>222</v>
       </c>
@@ -7671,10 +7944,22 @@
       </c>
       <c r="L139" s="5"/>
     </row>
-    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>222</v>
       </c>
+      <c r="B140" t="s">
+        <v>584</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D140" t="s">
+        <v>613</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F140" t="s">
         <v>268</v>
       </c>
@@ -7694,14 +7979,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="141" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B141" s="5"/>
-      <c r="C141" s="5"/>
-      <c r="D141" s="5"/>
-      <c r="E141" s="5"/>
+      <c r="B141" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F141" s="5" t="s">
         <v>546</v>
       </c>
@@ -7722,7 +8015,7 @@
       </c>
       <c r="L141" s="5"/>
     </row>
-    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>270</v>
       </c>
@@ -7745,7 +8038,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>270</v>
       </c>
@@ -7768,7 +8061,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>270</v>
       </c>
@@ -7791,7 +8084,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>270</v>
       </c>
@@ -7814,7 +8107,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>270</v>
       </c>
@@ -7837,7 +8130,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>270</v>
       </c>
@@ -7860,7 +8153,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>270</v>
       </c>
@@ -7883,7 +8176,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>270</v>
       </c>
@@ -7921,7 +8214,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>270</v>
       </c>
@@ -7959,7 +8252,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>270</v>
       </c>
@@ -7997,7 +8290,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>270</v>
       </c>
@@ -8032,7 +8325,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>270</v>
       </c>
@@ -8070,7 +8363,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>270</v>
       </c>
@@ -8093,7 +8386,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>270</v>
       </c>
@@ -8131,7 +8424,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>270</v>
       </c>
@@ -8169,7 +8462,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>270</v>
       </c>
@@ -8207,7 +8500,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" s="4" t="s">
         <v>270</v>
       </c>
@@ -8243,7 +8536,7 @@
       </c>
       <c r="L158" s="4"/>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
         <v>270</v>
       </c>
@@ -8281,7 +8574,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>270</v>
       </c>
@@ -8309,7 +8602,7 @@
       </c>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>270</v>
       </c>
@@ -8347,7 +8640,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>270</v>
       </c>
@@ -8385,7 +8678,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>270</v>
       </c>
@@ -8423,7 +8716,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
         <v>270</v>
       </c>
@@ -8459,7 +8752,7 @@
       </c>
       <c r="L164" s="4"/>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>270</v>
       </c>
@@ -8497,7 +8790,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
         <v>270</v>
       </c>
@@ -8525,7 +8818,7 @@
       </c>
       <c r="L166" s="4"/>
     </row>
-    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>270</v>
       </c>
@@ -8563,7 +8856,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>270</v>
       </c>
@@ -8601,7 +8894,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>270</v>
       </c>
@@ -8639,7 +8932,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A170" s="4" t="s">
         <v>270</v>
       </c>
@@ -8675,7 +8968,7 @@
       </c>
       <c r="L170" s="4"/>
     </row>
-    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>270</v>
       </c>
@@ -8713,7 +9006,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
         <v>270</v>
       </c>
@@ -8741,7 +9034,7 @@
       </c>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>270</v>
       </c>
@@ -8779,7 +9072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
         <v>270</v>
       </c>
@@ -8817,7 +9110,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>270</v>
       </c>
@@ -8855,7 +9148,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
         <v>270</v>
       </c>
@@ -8891,7 +9184,7 @@
       </c>
       <c r="L176" s="4"/>
     </row>
-    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>270</v>
       </c>
@@ -8929,7 +9222,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>364</v>
       </c>
@@ -8955,7 +9248,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
         <v>364</v>
       </c>
@@ -8985,7 +9278,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>64</v>
       </c>
@@ -9020,7 +9313,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>64</v>
       </c>
@@ -9055,7 +9348,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>379</v>
       </c>
@@ -9078,7 +9371,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="183" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>379</v>
       </c>
@@ -9104,7 +9397,7 @@
       </c>
       <c r="L183" s="5"/>
     </row>
-    <row r="184" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
         <v>379</v>
       </c>
@@ -9128,7 +9421,7 @@
       <c r="K184" s="5"/>
       <c r="L184" s="5"/>
     </row>
-    <row r="185" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>379</v>
       </c>
@@ -9221,7 +9514,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>183</v>
       </c>
@@ -9256,7 +9549,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="189" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
         <v>183</v>
       </c>
@@ -9292,10 +9585,22 @@
       </c>
       <c r="L189" s="5"/>
     </row>
-    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>183</v>
       </c>
+      <c r="B190" t="s">
+        <v>584</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D190" t="s">
+        <v>12</v>
+      </c>
+      <c r="E190" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F190" t="s">
         <v>396</v>
       </c>
@@ -9315,10 +9620,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="191" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
         <v>183</v>
       </c>
+      <c r="B191" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D191" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F191" s="2" t="s">
         <v>556</v>
       </c>
@@ -9338,7 +9655,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>183</v>
       </c>
@@ -9373,7 +9690,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="193" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
         <v>183</v>
       </c>
@@ -9408,10 +9725,22 @@
         <v>600</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>183</v>
       </c>
+      <c r="B194" t="s">
+        <v>584</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D194" t="s">
+        <v>614</v>
+      </c>
+      <c r="E194" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F194" t="s">
         <v>402</v>
       </c>
@@ -9431,14 +9760,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="195" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B195" s="5"/>
-      <c r="C195" s="5"/>
-      <c r="D195" s="5"/>
-      <c r="E195" s="5"/>
+      <c r="B195" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="E195" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F195" s="5" t="s">
         <v>558</v>
       </c>
@@ -9459,7 +9796,7 @@
       </c>
       <c r="L195" s="5"/>
     </row>
-    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>183</v>
       </c>
@@ -9494,7 +9831,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="197" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
         <v>183</v>
       </c>
@@ -9530,10 +9867,22 @@
       </c>
       <c r="L197" s="5"/>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>183</v>
       </c>
+      <c r="B198" t="s">
+        <v>584</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D198" t="s">
+        <v>614</v>
+      </c>
+      <c r="E198" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F198" t="s">
         <v>407</v>
       </c>
@@ -9553,14 +9902,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="199" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B199" s="5"/>
-      <c r="C199" s="5"/>
-      <c r="D199" s="5"/>
-      <c r="E199" s="5"/>
+      <c r="B199" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D199" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F199" s="5" t="s">
         <v>560</v>
       </c>
@@ -9581,7 +9938,7 @@
       </c>
       <c r="L199" s="5"/>
     </row>
-    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" s="4" t="s">
         <v>422</v>
       </c>
@@ -9617,7 +9974,7 @@
       </c>
       <c r="L200" s="4"/>
     </row>
-    <row r="201" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
         <v>422</v>
       </c>
@@ -9652,14 +10009,22 @@
         <v>600</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="B202" s="4"/>
-      <c r="C202" s="4"/>
-      <c r="D202" s="4"/>
-      <c r="E202" s="4"/>
+      <c r="B202" t="s">
+        <v>584</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="E202" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="F202" s="4" t="s">
         <v>411</v>
       </c>
@@ -9680,10 +10045,22 @@
       </c>
       <c r="L202" s="4"/>
     </row>
-    <row r="203" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
         <v>422</v>
       </c>
+      <c r="B203" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F203" s="2" t="s">
         <v>562</v>
       </c>
@@ -9703,7 +10080,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="204" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
         <v>422</v>
       </c>
@@ -9741,7 +10118,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="205" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
         <v>422</v>
       </c>
@@ -9779,7 +10156,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="206" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
         <v>422</v>
       </c>
@@ -9817,7 +10194,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="207" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
         <v>422</v>
       </c>
@@ -9855,7 +10232,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="208" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A208" s="2" t="s">
         <v>422</v>
       </c>
@@ -9893,7 +10270,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="209" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A209" s="2" t="s">
         <v>422</v>
       </c>
@@ -9931,7 +10308,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="210" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A210" s="2" t="s">
         <v>422</v>
       </c>
@@ -9966,7 +10343,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="211" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
         <v>422</v>
       </c>
@@ -10001,10 +10378,22 @@
         <v>600</v>
       </c>
     </row>
-    <row r="212" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
         <v>422</v>
       </c>
+      <c r="B212" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F212" s="2" t="s">
         <v>434</v>
       </c>
@@ -10024,10 +10413,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="213" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
         <v>422</v>
       </c>
+      <c r="B213" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F213" s="2" t="s">
         <v>486</v>
       </c>
@@ -10047,7 +10448,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="214" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
         <v>422</v>
       </c>
@@ -10082,7 +10483,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="215" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
         <v>422</v>
       </c>
@@ -10117,10 +10518,22 @@
         <v>600</v>
       </c>
     </row>
-    <row r="216" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>422</v>
       </c>
+      <c r="B216" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="E216" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F216" s="2" t="s">
         <v>441</v>
       </c>
@@ -10140,10 +10553,22 @@
         <v>601</v>
       </c>
     </row>
-    <row r="217" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>422</v>
       </c>
+      <c r="B217" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="E217" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="F217" s="2" t="s">
         <v>487</v>
       </c>
@@ -10163,7 +10588,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="218" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A218" s="2" t="s">
         <v>422</v>
       </c>
@@ -10201,7 +10626,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="219" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A219" s="2" t="s">
         <v>422</v>
       </c>
@@ -10239,7 +10664,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="220" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A220" s="2" t="s">
         <v>422</v>
       </c>
@@ -10277,7 +10702,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="221" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A221" s="5" t="s">
         <v>422</v>
       </c>
@@ -10315,7 +10740,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="222" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
         <v>422</v>
       </c>
@@ -10353,7 +10778,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="223" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A223" s="5" t="s">
         <v>422</v>
       </c>
@@ -10461,7 +10886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>364</v>
       </c>
@@ -10485,13 +10910,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L226" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="General Descriptive"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L226" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
begin work on health summary script
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-Toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B81CCDC-3674-4290-AE38-A2DDC50A7909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5DE0EA-981E-424F-A100-95304018D76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
@@ -351,7 +351,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2801" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2844" uniqueCount="899">
   <si>
     <t>Statistic Category</t>
   </si>
@@ -3045,6 +3045,9 @@
   </si>
   <si>
     <t>RECON_REPORT</t>
+  </si>
+  <si>
+    <t>forest_calcs.top5_ov_sp_level</t>
   </si>
 </sst>
 </file>
@@ -3666,8 +3669,8 @@
   <dimension ref="A1:M236"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C148" sqref="C148"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7289,7 +7292,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>173</v>
       </c>
@@ -7330,7 +7333,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>173</v>
       </c>
@@ -7371,7 +7374,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>173</v>
       </c>
@@ -7412,7 +7415,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>173</v>
       </c>
@@ -7450,7 +7453,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="97" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>173</v>
       </c>
@@ -7488,7 +7491,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>173</v>
       </c>
@@ -7529,7 +7532,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>173</v>
       </c>
@@ -7570,7 +7573,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>173</v>
       </c>
@@ -7611,7 +7614,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>173</v>
       </c>
@@ -7649,7 +7652,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>173</v>
       </c>
@@ -7688,7 +7691,7 @@
       </c>
       <c r="M102" s="5"/>
     </row>
-    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>173</v>
       </c>
@@ -7729,7 +7732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>173</v>
       </c>
@@ -7770,7 +7773,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>173</v>
       </c>
@@ -7811,7 +7814,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>173</v>
       </c>
@@ -7849,7 +7852,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="107" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>173</v>
       </c>
@@ -7887,7 +7890,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>173</v>
       </c>
@@ -7928,7 +7931,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>173</v>
       </c>
@@ -7969,7 +7972,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>173</v>
       </c>
@@ -8010,7 +8013,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>173</v>
       </c>
@@ -8048,7 +8051,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="112" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>173</v>
       </c>
@@ -8087,7 +8090,7 @@
       </c>
       <c r="M112" s="5"/>
     </row>
-    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>173</v>
       </c>
@@ -9222,7 +9225,7 @@
       </c>
       <c r="M141" s="5"/>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>249</v>
       </c>
@@ -9248,7 +9251,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>249</v>
       </c>
@@ -9274,7 +9277,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>249</v>
       </c>
@@ -9300,7 +9303,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>249</v>
       </c>
@@ -9326,7 +9329,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>249</v>
       </c>
@@ -9352,7 +9355,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>249</v>
       </c>
@@ -9378,10 +9381,13 @@
         <v>253</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>249</v>
       </c>
+      <c r="D148" t="s">
+        <v>12</v>
+      </c>
       <c r="F148" t="s">
         <v>779</v>
       </c>
@@ -9404,7 +9410,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>249</v>
       </c>
@@ -9412,7 +9418,7 @@
         <v>506</v>
       </c>
       <c r="C149" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D149" t="s">
         <v>541</v>
@@ -9445,7 +9451,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>249</v>
       </c>
@@ -9453,7 +9459,7 @@
         <v>506</v>
       </c>
       <c r="C150" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D150" t="s">
         <v>541</v>
@@ -9486,7 +9492,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>249</v>
       </c>
@@ -9494,7 +9500,7 @@
         <v>506</v>
       </c>
       <c r="C151" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D151" t="s">
         <v>541</v>
@@ -9527,7 +9533,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>249</v>
       </c>
@@ -9535,7 +9541,7 @@
         <v>506</v>
       </c>
       <c r="C152" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D152" t="s">
         <v>541</v>
@@ -9565,7 +9571,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>249</v>
       </c>
@@ -9573,7 +9579,7 @@
         <v>506</v>
       </c>
       <c r="C153" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D153" t="s">
         <v>541</v>
@@ -9606,10 +9612,19 @@
         <v>279</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>249</v>
       </c>
+      <c r="B154" t="s">
+        <v>506</v>
+      </c>
+      <c r="C154" t="s">
+        <v>898</v>
+      </c>
+      <c r="D154" t="s">
+        <v>541</v>
+      </c>
       <c r="E154" t="s">
         <v>516</v>
       </c>
@@ -9632,10 +9647,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>249</v>
       </c>
+      <c r="B155" t="s">
+        <v>506</v>
+      </c>
+      <c r="C155" t="s">
+        <v>898</v>
+      </c>
+      <c r="D155" t="s">
+        <v>541</v>
+      </c>
       <c r="E155" t="s">
         <v>516</v>
       </c>
@@ -9658,10 +9682,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>249</v>
       </c>
+      <c r="B156" t="s">
+        <v>506</v>
+      </c>
+      <c r="C156" t="s">
+        <v>898</v>
+      </c>
+      <c r="D156" t="s">
+        <v>12</v>
+      </c>
       <c r="F156" t="s">
         <v>811</v>
       </c>
@@ -9684,7 +9717,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>249</v>
       </c>
@@ -9692,7 +9725,7 @@
         <v>506</v>
       </c>
       <c r="C157" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D157" t="s">
         <v>542</v>
@@ -9725,7 +9758,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>249</v>
       </c>
@@ -9733,7 +9766,7 @@
         <v>506</v>
       </c>
       <c r="C158" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D158" t="s">
         <v>542</v>
@@ -9766,7 +9799,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>249</v>
       </c>
@@ -9774,7 +9807,7 @@
         <v>506</v>
       </c>
       <c r="C159" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D159" t="s">
         <v>542</v>
@@ -9807,7 +9840,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>249</v>
       </c>
@@ -9815,7 +9848,7 @@
         <v>506</v>
       </c>
       <c r="C160" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D160" t="s">
         <v>542</v>
@@ -9846,7 +9879,7 @@
       </c>
       <c r="M160" s="4"/>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>249</v>
       </c>
@@ -9854,7 +9887,7 @@
         <v>506</v>
       </c>
       <c r="C161" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D161" t="s">
         <v>542</v>
@@ -9887,10 +9920,19 @@
         <v>293</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>249</v>
       </c>
+      <c r="B162" t="s">
+        <v>506</v>
+      </c>
+      <c r="C162" t="s">
+        <v>898</v>
+      </c>
+      <c r="D162" t="s">
+        <v>542</v>
+      </c>
       <c r="E162" t="s">
         <v>516</v>
       </c>
@@ -9913,10 +9955,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>249</v>
       </c>
+      <c r="B163" t="s">
+        <v>506</v>
+      </c>
+      <c r="C163" t="s">
+        <v>898</v>
+      </c>
+      <c r="D163" t="s">
+        <v>542</v>
+      </c>
       <c r="E163" t="s">
         <v>516</v>
       </c>
@@ -9939,13 +9990,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B164" s="4"/>
-      <c r="C164" s="4"/>
-      <c r="D164" s="4"/>
+      <c r="B164" t="s">
+        <v>506</v>
+      </c>
+      <c r="C164" t="s">
+        <v>898</v>
+      </c>
+      <c r="D164" t="s">
+        <v>12</v>
+      </c>
       <c r="E164" s="4"/>
       <c r="F164" t="s">
         <v>806</v>
@@ -9970,7 +10027,7 @@
       </c>
       <c r="M164" s="4"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>249</v>
       </c>
@@ -9978,7 +10035,7 @@
         <v>506</v>
       </c>
       <c r="C165" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D165" t="s">
         <v>543</v>
@@ -10011,7 +10068,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>249</v>
       </c>
@@ -10019,7 +10076,7 @@
         <v>506</v>
       </c>
       <c r="C166" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D166" t="s">
         <v>543</v>
@@ -10052,7 +10109,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>249</v>
       </c>
@@ -10060,7 +10117,7 @@
         <v>506</v>
       </c>
       <c r="C167" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D167" t="s">
         <v>543</v>
@@ -10093,7 +10150,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>249</v>
       </c>
@@ -10101,7 +10158,7 @@
         <v>506</v>
       </c>
       <c r="C168" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D168" t="s">
         <v>543</v>
@@ -10132,7 +10189,7 @@
       </c>
       <c r="M168" s="4"/>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>249</v>
       </c>
@@ -10140,7 +10197,7 @@
         <v>506</v>
       </c>
       <c r="C169" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D169" t="s">
         <v>543</v>
@@ -10173,10 +10230,19 @@
         <v>293</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>249</v>
       </c>
+      <c r="B170" t="s">
+        <v>506</v>
+      </c>
+      <c r="C170" t="s">
+        <v>898</v>
+      </c>
+      <c r="D170" t="s">
+        <v>543</v>
+      </c>
       <c r="E170" t="s">
         <v>516</v>
       </c>
@@ -10199,10 +10265,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>249</v>
       </c>
+      <c r="B171" t="s">
+        <v>506</v>
+      </c>
+      <c r="C171" t="s">
+        <v>898</v>
+      </c>
+      <c r="D171" t="s">
+        <v>543</v>
+      </c>
       <c r="E171" t="s">
         <v>516</v>
       </c>
@@ -10225,13 +10300,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B172" s="4"/>
-      <c r="C172" s="4"/>
-      <c r="D172" s="4"/>
+      <c r="B172" t="s">
+        <v>506</v>
+      </c>
+      <c r="C172" t="s">
+        <v>898</v>
+      </c>
+      <c r="D172" t="s">
+        <v>12</v>
+      </c>
       <c r="E172" s="4"/>
       <c r="F172" t="s">
         <v>801</v>
@@ -10256,7 +10337,7 @@
       </c>
       <c r="M172" s="4"/>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>249</v>
       </c>
@@ -10264,7 +10345,7 @@
         <v>506</v>
       </c>
       <c r="C173" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D173" t="s">
         <v>544</v>
@@ -10297,7 +10378,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>249</v>
       </c>
@@ -10305,7 +10386,7 @@
         <v>506</v>
       </c>
       <c r="C174" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D174" t="s">
         <v>544</v>
@@ -10338,7 +10419,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>249</v>
       </c>
@@ -10346,7 +10427,7 @@
         <v>506</v>
       </c>
       <c r="C175" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D175" t="s">
         <v>544</v>
@@ -10379,7 +10460,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>249</v>
       </c>
@@ -10387,7 +10468,7 @@
         <v>506</v>
       </c>
       <c r="C176" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D176" t="s">
         <v>544</v>
@@ -10418,7 +10499,7 @@
       </c>
       <c r="M176" s="4"/>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>249</v>
       </c>
@@ -10426,7 +10507,7 @@
         <v>506</v>
       </c>
       <c r="C177" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D177" t="s">
         <v>544</v>
@@ -10459,10 +10540,19 @@
         <v>293</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>249</v>
       </c>
+      <c r="B178" t="s">
+        <v>506</v>
+      </c>
+      <c r="C178" t="s">
+        <v>898</v>
+      </c>
+      <c r="D178" t="s">
+        <v>544</v>
+      </c>
       <c r="E178" t="s">
         <v>516</v>
       </c>
@@ -10485,10 +10575,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>249</v>
       </c>
+      <c r="B179" t="s">
+        <v>506</v>
+      </c>
+      <c r="C179" t="s">
+        <v>898</v>
+      </c>
+      <c r="D179" t="s">
+        <v>544</v>
+      </c>
       <c r="E179" t="s">
         <v>516</v>
       </c>
@@ -10511,13 +10610,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B180" s="4"/>
-      <c r="C180" s="4"/>
-      <c r="D180" s="4"/>
+      <c r="B180" t="s">
+        <v>506</v>
+      </c>
+      <c r="C180" t="s">
+        <v>898</v>
+      </c>
+      <c r="D180" t="s">
+        <v>12</v>
+      </c>
       <c r="E180" s="4"/>
       <c r="F180" t="s">
         <v>843</v>
@@ -10542,7 +10647,7 @@
       </c>
       <c r="M180" s="4"/>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>249</v>
       </c>
@@ -10550,7 +10655,7 @@
         <v>506</v>
       </c>
       <c r="C181" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D181" t="s">
         <v>545</v>
@@ -10583,7 +10688,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
         <v>249</v>
       </c>
@@ -10591,7 +10696,7 @@
         <v>506</v>
       </c>
       <c r="C182" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D182" t="s">
         <v>545</v>
@@ -10624,7 +10729,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>249</v>
       </c>
@@ -10632,7 +10737,7 @@
         <v>506</v>
       </c>
       <c r="C183" t="s">
-        <v>514</v>
+        <v>898</v>
       </c>
       <c r="D183" t="s">
         <v>545</v>
@@ -10665,7 +10770,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
         <v>249</v>
       </c>
@@ -10673,7 +10778,7 @@
         <v>506</v>
       </c>
       <c r="C184" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D184" t="s">
         <v>545</v>
@@ -10704,7 +10809,7 @@
       </c>
       <c r="M184" s="4"/>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>249</v>
       </c>
@@ -10712,7 +10817,7 @@
         <v>506</v>
       </c>
       <c r="C185" t="s">
-        <v>521</v>
+        <v>898</v>
       </c>
       <c r="D185" t="s">
         <v>545</v>
@@ -10745,10 +10850,19 @@
         <v>293</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>249</v>
       </c>
+      <c r="B186" t="s">
+        <v>506</v>
+      </c>
+      <c r="C186" t="s">
+        <v>898</v>
+      </c>
+      <c r="D186" t="s">
+        <v>545</v>
+      </c>
       <c r="E186" t="s">
         <v>516</v>
       </c>
@@ -10771,9 +10885,18 @@
         <v>78</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>249</v>
+      </c>
+      <c r="B187" t="s">
+        <v>506</v>
+      </c>
+      <c r="C187" t="s">
+        <v>898</v>
+      </c>
+      <c r="D187" t="s">
+        <v>545</v>
       </c>
       <c r="E187" t="s">
         <v>516</v>
@@ -11119,7 +11242,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>173</v>
       </c>
@@ -11157,7 +11280,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="199" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>173</v>
       </c>
@@ -11196,7 +11319,7 @@
       </c>
       <c r="M199" s="5"/>
     </row>
-    <row r="200" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>173</v>
       </c>
@@ -11234,7 +11357,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="201" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>173</v>
       </c>
@@ -11272,7 +11395,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="202" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>173</v>
       </c>
@@ -11310,7 +11433,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="203" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>173</v>
       </c>
@@ -11348,7 +11471,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="204" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>173</v>
       </c>
@@ -11386,7 +11509,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="205" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>173</v>
       </c>
@@ -11425,7 +11548,7 @@
       </c>
       <c r="M205" s="5"/>
     </row>
-    <row r="206" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>173</v>
       </c>
@@ -11463,7 +11586,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="207" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>173</v>
       </c>
@@ -11502,7 +11625,7 @@
       </c>
       <c r="M207" s="5"/>
     </row>
-    <row r="208" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>173</v>
       </c>
@@ -11540,7 +11663,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="209" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>173</v>
       </c>
@@ -12635,7 +12758,7 @@
   <autoFilter ref="A1:M236" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Species"/>
+        <filter val="Health"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
updated forest calc functions and continued health script
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-Toolbox\fmgpy\summaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5DE0EA-981E-424F-A100-95304018D76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64AF1A4-A721-4072-BDC9-1B2B36A4F13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
+    <workbookView xWindow="39460" yWindow="900" windowWidth="36220" windowHeight="18850" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="One To One" sheetId="1" r:id="rId1"/>
@@ -3670,27 +3670,27 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
+      <selection pane="bottomLeft" activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" customWidth="1"/>
+    <col min="3" max="3" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="51.42578125" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="81.42578125" customWidth="1"/>
-    <col min="10" max="10" width="59.85546875" customWidth="1"/>
-    <col min="11" max="11" width="53.140625" customWidth="1"/>
-    <col min="12" max="12" width="32.5703125" customWidth="1"/>
-    <col min="13" max="13" width="91.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.453125" customWidth="1"/>
+    <col min="8" max="8" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="81.453125" customWidth="1"/>
+    <col min="10" max="10" width="59.81640625" customWidth="1"/>
+    <col min="11" max="11" width="53.1796875" customWidth="1"/>
+    <col min="12" max="12" width="32.54296875" customWidth="1"/>
+    <col min="13" max="13" width="91.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -3982,7 +3982,7 @@
       </c>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -4283,7 +4283,7 @@
       </c>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
@@ -4431,7 +4431,7 @@
       </c>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -4506,7 +4506,7 @@
       </c>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>64</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
@@ -4888,7 +4888,7 @@
       </c>
       <c r="M32" s="5"/>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>85</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>85</v>
       </c>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>85</v>
       </c>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>85</v>
       </c>
@@ -5166,7 +5166,7 @@
       </c>
       <c r="M39" s="5"/>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>85</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>85</v>
       </c>
@@ -5451,7 +5451,7 @@
       </c>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>85</v>
       </c>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="M47" s="5"/>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="M49" s="5"/>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>85</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>85</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>85</v>
       </c>
@@ -5890,7 +5890,7 @@
       </c>
       <c r="M57" s="5"/>
     </row>
-    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>85</v>
       </c>
@@ -5929,7 +5929,7 @@
       </c>
       <c r="M58" s="4"/>
     </row>
-    <row r="59" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>85</v>
       </c>
@@ -5968,7 +5968,7 @@
       </c>
       <c r="M59" s="5"/>
     </row>
-    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>85</v>
       </c>
@@ -6009,7 +6009,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>85</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>85</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>85</v>
       </c>
@@ -6367,7 +6367,7 @@
       </c>
       <c r="M69" s="5"/>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>85</v>
       </c>
@@ -6690,7 +6690,7 @@
       </c>
       <c r="M77" s="5"/>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>85</v>
       </c>
@@ -6767,7 +6767,7 @@
       </c>
       <c r="M79" s="5"/>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>85</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>85</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>85</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>85</v>
       </c>
@@ -7052,7 +7052,7 @@
       </c>
       <c r="M86" s="5"/>
     </row>
-    <row r="87" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>85</v>
       </c>
@@ -7091,7 +7091,7 @@
       </c>
       <c r="M87" s="5"/>
     </row>
-    <row r="88" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>85</v>
       </c>
@@ -7130,7 +7130,7 @@
       </c>
       <c r="M88" s="5"/>
     </row>
-    <row r="89" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>85</v>
       </c>
@@ -7169,7 +7169,7 @@
       </c>
       <c r="M89" s="5"/>
     </row>
-    <row r="90" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>85</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>85</v>
       </c>
@@ -7251,7 +7251,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>85</v>
       </c>
@@ -7292,7 +7292,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>173</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>173</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>173</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>173</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="97" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>173</v>
       </c>
@@ -7491,7 +7491,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>173</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>173</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>173</v>
       </c>
@@ -7614,7 +7614,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>173</v>
       </c>
@@ -7652,7 +7652,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>173</v>
       </c>
@@ -7691,7 +7691,7 @@
       </c>
       <c r="M102" s="5"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>173</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>173</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>173</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>173</v>
       </c>
@@ -7852,7 +7852,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="107" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>173</v>
       </c>
@@ -7890,7 +7890,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>173</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>173</v>
       </c>
@@ -7972,7 +7972,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>173</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>173</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="112" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>173</v>
       </c>
@@ -8090,7 +8090,7 @@
       </c>
       <c r="M112" s="5"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>173</v>
       </c>
@@ -8119,7 +8119,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>208</v>
       </c>
@@ -8160,7 +8160,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>208</v>
       </c>
@@ -8201,7 +8201,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>208</v>
       </c>
@@ -8242,7 +8242,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>208</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="118" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>208</v>
       </c>
@@ -8318,7 +8318,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>208</v>
       </c>
@@ -8357,7 +8357,7 @@
       </c>
       <c r="M119" s="4"/>
     </row>
-    <row r="120" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>208</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>208</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>208</v>
       </c>
@@ -8477,7 +8477,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>208</v>
       </c>
@@ -8518,7 +8518,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>208</v>
       </c>
@@ -8557,7 +8557,7 @@
       </c>
       <c r="M124" s="4"/>
     </row>
-    <row r="125" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>208</v>
       </c>
@@ -8595,7 +8595,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>208</v>
       </c>
@@ -8634,7 +8634,7 @@
       </c>
       <c r="M126" s="4"/>
     </row>
-    <row r="127" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>208</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>208</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>208</v>
       </c>
@@ -8754,7 +8754,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>208</v>
       </c>
@@ -8795,7 +8795,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>208</v>
       </c>
@@ -8833,7 +8833,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="132" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>208</v>
       </c>
@@ -8871,7 +8871,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>208</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="134" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>208</v>
       </c>
@@ -8948,7 +8948,7 @@
       </c>
       <c r="M134" s="5"/>
     </row>
-    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>208</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>208</v>
       </c>
@@ -9030,7 +9030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>208</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>208</v>
       </c>
@@ -9109,7 +9109,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="139" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>208</v>
       </c>
@@ -9148,7 +9148,7 @@
       </c>
       <c r="M139" s="5"/>
     </row>
-    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>208</v>
       </c>
@@ -9186,7 +9186,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="141" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>208</v>
       </c>
@@ -9225,7 +9225,7 @@
       </c>
       <c r="M141" s="5"/>
     </row>
-    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>249</v>
       </c>
@@ -9251,7 +9251,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>249</v>
       </c>
@@ -9277,7 +9277,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>249</v>
       </c>
@@ -9303,7 +9303,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>249</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>249</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>249</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>249</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>249</v>
       </c>
@@ -9451,7 +9451,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>249</v>
       </c>
@@ -9492,7 +9492,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>249</v>
       </c>
@@ -9533,7 +9533,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>249</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>249</v>
       </c>
@@ -9612,7 +9612,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>249</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>249</v>
       </c>
@@ -9682,7 +9682,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>249</v>
       </c>
@@ -9717,7 +9717,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>249</v>
       </c>
@@ -9758,7 +9758,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>249</v>
       </c>
@@ -9799,7 +9799,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>249</v>
       </c>
@@ -9840,7 +9840,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>249</v>
       </c>
@@ -9879,7 +9879,7 @@
       </c>
       <c r="M160" s="4"/>
     </row>
-    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
         <v>249</v>
       </c>
@@ -9920,7 +9920,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>249</v>
       </c>
@@ -9955,7 +9955,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>249</v>
       </c>
@@ -9990,7 +9990,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
         <v>249</v>
       </c>
@@ -10027,7 +10027,7 @@
       </c>
       <c r="M164" s="4"/>
     </row>
-    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>249</v>
       </c>
@@ -10068,7 +10068,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>249</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>249</v>
       </c>
@@ -10150,7 +10150,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>249</v>
       </c>
@@ -10189,7 +10189,7 @@
       </c>
       <c r="M168" s="4"/>
     </row>
-    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>249</v>
       </c>
@@ -10230,7 +10230,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>249</v>
       </c>
@@ -10265,7 +10265,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>249</v>
       </c>
@@ -10300,7 +10300,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
         <v>249</v>
       </c>
@@ -10337,7 +10337,7 @@
       </c>
       <c r="M172" s="4"/>
     </row>
-    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>249</v>
       </c>
@@ -10378,7 +10378,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
         <v>249</v>
       </c>
@@ -10419,7 +10419,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>249</v>
       </c>
@@ -10460,7 +10460,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
         <v>249</v>
       </c>
@@ -10499,7 +10499,7 @@
       </c>
       <c r="M176" s="4"/>
     </row>
-    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>249</v>
       </c>
@@ -10540,7 +10540,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>249</v>
       </c>
@@ -10575,7 +10575,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>249</v>
       </c>
@@ -10610,7 +10610,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="4" t="s">
         <v>249</v>
       </c>
@@ -10647,7 +10647,7 @@
       </c>
       <c r="M180" s="4"/>
     </row>
-    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>249</v>
       </c>
@@ -10688,7 +10688,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="4" t="s">
         <v>249</v>
       </c>
@@ -10729,7 +10729,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>249</v>
       </c>
@@ -10770,7 +10770,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="4" t="s">
         <v>249</v>
       </c>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="M184" s="4"/>
     </row>
-    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>249</v>
       </c>
@@ -10850,7 +10850,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>249</v>
       </c>
@@ -10885,7 +10885,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>249</v>
       </c>
@@ -10920,7 +10920,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="188" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>333</v>
       </c>
@@ -10949,7 +10949,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="189" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="4" t="s">
         <v>333</v>
       </c>
@@ -10982,7 +10982,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>64</v>
       </c>
@@ -11020,7 +11020,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>64</v>
       </c>
@@ -11058,7 +11058,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>348</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="193" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" s="5" t="s">
         <v>348</v>
       </c>
@@ -11113,7 +11113,7 @@
       </c>
       <c r="M193" s="5"/>
     </row>
-    <row r="194" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
         <v>348</v>
       </c>
@@ -11140,7 +11140,7 @@
       <c r="L194" s="5"/>
       <c r="M194" s="5"/>
     </row>
-    <row r="195" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>348</v>
       </c>
@@ -11165,7 +11165,7 @@
       <c r="L195" s="5"/>
       <c r="M195" s="5"/>
     </row>
-    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" s="4" t="s">
         <v>8</v>
       </c>
@@ -11204,7 +11204,7 @@
       </c>
       <c r="M196" s="4"/>
     </row>
-    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>8</v>
       </c>
@@ -11242,7 +11242,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>173</v>
       </c>
@@ -11280,7 +11280,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="199" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>173</v>
       </c>
@@ -11319,7 +11319,7 @@
       </c>
       <c r="M199" s="5"/>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>173</v>
       </c>
@@ -11357,7 +11357,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="201" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
         <v>173</v>
       </c>
@@ -11395,7 +11395,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>173</v>
       </c>
@@ -11433,7 +11433,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="203" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
         <v>173</v>
       </c>
@@ -11471,7 +11471,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>173</v>
       </c>
@@ -11509,7 +11509,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="205" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A205" s="5" t="s">
         <v>173</v>
       </c>
@@ -11548,7 +11548,7 @@
       </c>
       <c r="M205" s="5"/>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>173</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="207" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A207" s="5" t="s">
         <v>173</v>
       </c>
@@ -11625,7 +11625,7 @@
       </c>
       <c r="M207" s="5"/>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>173</v>
       </c>
@@ -11663,7 +11663,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="209" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A209" s="5" t="s">
         <v>173</v>
       </c>
@@ -11702,7 +11702,7 @@
       </c>
       <c r="M209" s="5"/>
     </row>
-    <row r="210" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" s="4" t="s">
         <v>384</v>
       </c>
@@ -11741,7 +11741,7 @@
       </c>
       <c r="M210" s="4"/>
     </row>
-    <row r="211" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
         <v>384</v>
       </c>
@@ -11779,7 +11779,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="212" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" s="4" t="s">
         <v>384</v>
       </c>
@@ -11818,7 +11818,7 @@
       </c>
       <c r="M212" s="4"/>
     </row>
-    <row r="213" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
         <v>384</v>
       </c>
@@ -11856,7 +11856,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="214" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
         <v>384</v>
       </c>
@@ -11897,7 +11897,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="215" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
         <v>384</v>
       </c>
@@ -11938,7 +11938,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="216" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>384</v>
       </c>
@@ -11979,7 +11979,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="217" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>384</v>
       </c>
@@ -12020,7 +12020,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="218" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" s="2" t="s">
         <v>384</v>
       </c>
@@ -12061,7 +12061,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="219" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" s="2" t="s">
         <v>384</v>
       </c>
@@ -12102,7 +12102,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="220" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" s="2" t="s">
         <v>384</v>
       </c>
@@ -12140,7 +12140,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="221" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" s="2" t="s">
         <v>384</v>
       </c>
@@ -12178,7 +12178,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="222" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" s="2" t="s">
         <v>384</v>
       </c>
@@ -12216,7 +12216,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="223" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" s="2" t="s">
         <v>384</v>
       </c>
@@ -12254,7 +12254,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="224" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" s="2" t="s">
         <v>384</v>
       </c>
@@ -12292,7 +12292,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="225" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" s="2" t="s">
         <v>384</v>
       </c>
@@ -12330,7 +12330,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="226" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" s="2" t="s">
         <v>384</v>
       </c>
@@ -12368,7 +12368,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="227" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" s="2" t="s">
         <v>384</v>
       </c>
@@ -12406,7 +12406,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="228" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" s="2" t="s">
         <v>384</v>
       </c>
@@ -12447,7 +12447,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="229" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" s="2" t="s">
         <v>384</v>
       </c>
@@ -12488,7 +12488,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="230" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" s="2" t="s">
         <v>384</v>
       </c>
@@ -12529,7 +12529,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="231" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" s="5" t="s">
         <v>384</v>
       </c>
@@ -12570,7 +12570,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="232" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" s="5" t="s">
         <v>384</v>
       </c>
@@ -12611,7 +12611,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="233" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" s="5" t="s">
         <v>384</v>
       </c>
@@ -12652,7 +12652,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="234" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>8</v>
       </c>
@@ -12690,7 +12690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="235" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>8</v>
       </c>
@@ -12728,7 +12728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="236" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>333</v>
       </c>
@@ -12776,19 +12776,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="32.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.453125" customWidth="1"/>
+    <col min="7" max="7" width="31.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12814,12 +12814,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>501</v>
       </c>

</xml_diff>

<commit_message>
start vert comp summary
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02647197-85FF-434E-9934-33EAABC339B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6551F06-C610-4414-A068-47A5A2D5EB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1370" windowWidth="35280" windowHeight="20330" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
+    <workbookView xWindow="38860" yWindow="160" windowWidth="35280" windowHeight="20330" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="One To One" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2882" uniqueCount="906">
   <si>
     <t>Statistic Category</t>
   </si>
@@ -3068,7 +3068,7 @@
     <t>AGE_UND_COV</t>
   </si>
   <si>
-    <t>https://stackoverflow.com/questions/15222754/groupby-pandas-dataframe-and-select-most-common-value</t>
+    <t>forest_calcs.get_groupby_modes</t>
   </si>
 </sst>
 </file>
@@ -3690,15 +3690,15 @@
   <dimension ref="A1:M237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D146" sqref="D146"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F250" sqref="F250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.54296875" customWidth="1"/>
     <col min="2" max="2" width="25.81640625" customWidth="1"/>
-    <col min="3" max="3" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.1796875" customWidth="1"/>
     <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.54296875" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
@@ -9246,10 +9246,22 @@
       </c>
       <c r="M141" s="5"/>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>246</v>
       </c>
+      <c r="B142" t="s">
+        <v>501</v>
+      </c>
+      <c r="C142" t="s">
+        <v>905</v>
+      </c>
+      <c r="D142" t="s">
+        <v>12</v>
+      </c>
+      <c r="E142" t="s">
+        <v>511</v>
+      </c>
       <c r="F142" t="s">
         <v>748</v>
       </c>
@@ -9272,10 +9284,22 @@
         <v>250</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>246</v>
       </c>
+      <c r="B143" t="s">
+        <v>501</v>
+      </c>
+      <c r="C143" t="s">
+        <v>905</v>
+      </c>
+      <c r="D143" t="s">
+        <v>12</v>
+      </c>
+      <c r="E143" t="s">
+        <v>511</v>
+      </c>
       <c r="F143" t="s">
         <v>749</v>
       </c>
@@ -9298,13 +9322,22 @@
         <v>250</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>246</v>
       </c>
+      <c r="B144" t="s">
+        <v>501</v>
+      </c>
       <c r="C144" t="s">
         <v>905</v>
       </c>
+      <c r="D144" t="s">
+        <v>12</v>
+      </c>
+      <c r="E144" t="s">
+        <v>511</v>
+      </c>
       <c r="F144" t="s">
         <v>750</v>
       </c>
@@ -9327,10 +9360,22 @@
         <v>250</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>246</v>
       </c>
+      <c r="B145" t="s">
+        <v>501</v>
+      </c>
+      <c r="C145" t="s">
+        <v>905</v>
+      </c>
+      <c r="D145" t="s">
+        <v>12</v>
+      </c>
+      <c r="E145" t="s">
+        <v>511</v>
+      </c>
       <c r="F145" t="s">
         <v>751</v>
       </c>
@@ -9353,10 +9398,22 @@
         <v>250</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>246</v>
       </c>
+      <c r="B146" t="s">
+        <v>501</v>
+      </c>
+      <c r="C146" t="s">
+        <v>905</v>
+      </c>
+      <c r="D146" t="s">
+        <v>12</v>
+      </c>
+      <c r="E146" t="s">
+        <v>511</v>
+      </c>
       <c r="F146" t="s">
         <v>752</v>
       </c>
@@ -9379,10 +9436,22 @@
         <v>250</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>246</v>
       </c>
+      <c r="B147" t="s">
+        <v>501</v>
+      </c>
+      <c r="C147" t="s">
+        <v>905</v>
+      </c>
+      <c r="D147" t="s">
+        <v>12</v>
+      </c>
+      <c r="E147" t="s">
+        <v>511</v>
+      </c>
       <c r="F147" t="s">
         <v>753</v>
       </c>
@@ -9405,10 +9474,16 @@
         <v>250</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>246</v>
       </c>
+      <c r="B148" t="s">
+        <v>501</v>
+      </c>
+      <c r="C148" t="s">
+        <v>905</v>
+      </c>
       <c r="D148" t="s">
         <v>12</v>
       </c>
@@ -9434,7 +9509,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>246</v>
       </c>
@@ -9475,7 +9550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>246</v>
       </c>
@@ -9516,7 +9591,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>246</v>
       </c>
@@ -9557,7 +9632,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>246</v>
       </c>
@@ -9595,7 +9670,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>246</v>
       </c>
@@ -9636,7 +9711,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>246</v>
       </c>
@@ -9671,7 +9746,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>246</v>
       </c>
@@ -9706,7 +9781,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>246</v>
       </c>
@@ -9741,7 +9816,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>246</v>
       </c>
@@ -9782,7 +9857,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>246</v>
       </c>
@@ -9823,7 +9898,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>246</v>
       </c>
@@ -9864,7 +9939,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>246</v>
       </c>
@@ -9903,7 +9978,7 @@
       </c>
       <c r="M160" s="4"/>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
         <v>246</v>
       </c>
@@ -9944,7 +10019,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>246</v>
       </c>
@@ -9979,7 +10054,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>246</v>
       </c>
@@ -10014,7 +10089,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
         <v>246</v>
       </c>
@@ -10051,7 +10126,7 @@
       </c>
       <c r="M164" s="4"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>246</v>
       </c>
@@ -10092,7 +10167,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>246</v>
       </c>
@@ -10133,7 +10208,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>246</v>
       </c>
@@ -10174,7 +10249,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>246</v>
       </c>
@@ -10213,7 +10288,7 @@
       </c>
       <c r="M168" s="4"/>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>246</v>
       </c>
@@ -10254,7 +10329,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>246</v>
       </c>
@@ -10289,7 +10364,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>246</v>
       </c>
@@ -10324,7 +10399,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
         <v>246</v>
       </c>
@@ -10361,7 +10436,7 @@
       </c>
       <c r="M172" s="4"/>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>246</v>
       </c>
@@ -10402,7 +10477,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
         <v>246</v>
       </c>
@@ -10443,7 +10518,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>246</v>
       </c>
@@ -10484,7 +10559,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
         <v>246</v>
       </c>
@@ -10523,7 +10598,7 @@
       </c>
       <c r="M176" s="4"/>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>246</v>
       </c>
@@ -10564,7 +10639,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>246</v>
       </c>
@@ -10599,7 +10674,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>246</v>
       </c>
@@ -10634,7 +10709,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="4" t="s">
         <v>246</v>
       </c>
@@ -10671,7 +10746,7 @@
       </c>
       <c r="M180" s="4"/>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>246</v>
       </c>
@@ -10712,7 +10787,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="4" t="s">
         <v>246</v>
       </c>
@@ -10753,7 +10828,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>246</v>
       </c>
@@ -10794,7 +10869,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="4" t="s">
         <v>246</v>
       </c>
@@ -10833,7 +10908,7 @@
       </c>
       <c r="M184" s="4"/>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>246</v>
       </c>
@@ -10874,7 +10949,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>246</v>
       </c>
@@ -10909,7 +10984,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>246</v>
       </c>
@@ -11919,7 +11994,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="215" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
         <v>380</v>
       </c>
@@ -11960,7 +12035,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="216" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>380</v>
       </c>
@@ -12001,7 +12076,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="217" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>380</v>
       </c>
@@ -12042,7 +12117,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="218" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A218" s="2" t="s">
         <v>380</v>
       </c>
@@ -12083,7 +12158,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="219" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A219" s="2" t="s">
         <v>380</v>
       </c>
@@ -12124,7 +12199,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="220" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A220" s="2" t="s">
         <v>380</v>
       </c>
@@ -12469,7 +12544,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="229" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A229" s="2" t="s">
         <v>380</v>
       </c>
@@ -12510,7 +12585,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="230" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A230" s="2" t="s">
         <v>380</v>
       </c>
@@ -12551,7 +12626,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="231" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A231" s="2" t="s">
         <v>380</v>
       </c>
@@ -12592,7 +12667,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="232" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A232" s="5" t="s">
         <v>380</v>
       </c>
@@ -12633,7 +12708,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="233" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A233" s="5" t="s">
         <v>380</v>
       </c>
@@ -12674,7 +12749,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="234" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A234" s="5" t="s">
         <v>380</v>
       </c>
@@ -12821,7 +12896,12 @@
   <autoFilter ref="A1:M237" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Species"/>
+        <filter val="Vertical Composition"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="forest_calcs.TPA_BA_QMDBH_Plot &amp; Level"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
wrote vert comp summary, needs debug
</commit_message>
<xml_diff>
--- a/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
+++ b/fmgpy/summaries/FMG_SummaryCodeRewrite_ProposedStatistics_1to1_20220920.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-toolbox\fmgpy\summaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalProjects\FMG\FMG-Toolbox\fmgpy\summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6551F06-C610-4414-A068-47A5A2D5EB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0AFF22-A9C1-4F71-9799-BC226AF43D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38860" yWindow="160" windowWidth="35280" windowHeight="20330" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
+    <workbookView xWindow="2685" yWindow="195" windowWidth="25620" windowHeight="13875" xr2:uid="{966A738F-9F83-430B-83ED-A457BA229C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="One To One" sheetId="1" r:id="rId1"/>
@@ -3690,28 +3690,28 @@
   <dimension ref="A1:M237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F250" sqref="F250"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G188" sqref="G188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" customWidth="1"/>
-    <col min="2" max="2" width="25.81640625" customWidth="1"/>
-    <col min="3" max="3" width="45.1796875" customWidth="1"/>
-    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="58.26953125" customWidth="1"/>
-    <col min="8" max="8" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="81.453125" customWidth="1"/>
-    <col min="10" max="10" width="59.81640625" customWidth="1"/>
-    <col min="11" max="11" width="53.1796875" customWidth="1"/>
-    <col min="12" max="12" width="32.54296875" customWidth="1"/>
-    <col min="13" max="13" width="91.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="84.42578125" customWidth="1"/>
+    <col min="10" max="10" width="59.85546875" customWidth="1"/>
+    <col min="11" max="11" width="53.140625" customWidth="1"/>
+    <col min="12" max="12" width="32.5703125" customWidth="1"/>
+    <col min="13" max="13" width="91.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -3859,7 +3859,7 @@
       </c>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -4003,7 +4003,7 @@
       </c>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -4080,7 +4080,7 @@
       </c>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -4119,7 +4119,7 @@
       </c>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -4304,7 +4304,7 @@
       </c>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
@@ -4452,7 +4452,7 @@
       </c>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -4527,7 +4527,7 @@
       </c>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>64</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="M32" s="5"/>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>82</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>82</v>
       </c>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>82</v>
       </c>
@@ -5148,7 +5148,7 @@
       </c>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>82</v>
       </c>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="M39" s="5"/>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>82</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>82</v>
       </c>
@@ -5472,7 +5472,7 @@
       </c>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>82</v>
       </c>
@@ -5511,7 +5511,7 @@
       </c>
       <c r="M47" s="5"/>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>82</v>
       </c>
@@ -5588,7 +5588,7 @@
       </c>
       <c r="M49" s="5"/>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>82</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>82</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>82</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>82</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>82</v>
       </c>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="M57" s="5"/>
     </row>
-    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>82</v>
       </c>
@@ -5950,7 +5950,7 @@
       </c>
       <c r="M58" s="4"/>
     </row>
-    <row r="59" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>82</v>
       </c>
@@ -5989,7 +5989,7 @@
       </c>
       <c r="M59" s="5"/>
     </row>
-    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>82</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>82</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>82</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>82</v>
       </c>
@@ -6388,7 +6388,7 @@
       </c>
       <c r="M69" s="5"/>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -6672,7 +6672,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>82</v>
       </c>
@@ -6711,7 +6711,7 @@
       </c>
       <c r="M77" s="5"/>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -6749,7 +6749,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>82</v>
       </c>
@@ -6788,7 +6788,7 @@
       </c>
       <c r="M79" s="5"/>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>82</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="84" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>82</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>82</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>82</v>
       </c>
@@ -7073,7 +7073,7 @@
       </c>
       <c r="M86" s="5"/>
     </row>
-    <row r="87" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>82</v>
       </c>
@@ -7112,7 +7112,7 @@
       </c>
       <c r="M87" s="5"/>
     </row>
-    <row r="88" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>82</v>
       </c>
@@ -7151,7 +7151,7 @@
       </c>
       <c r="M88" s="5"/>
     </row>
-    <row r="89" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>82</v>
       </c>
@@ -7190,7 +7190,7 @@
       </c>
       <c r="M89" s="5"/>
     </row>
-    <row r="90" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>82</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>82</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="92" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>82</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>170</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>170</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>170</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>170</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="97" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>170</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>170</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>170</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>170</v>
       </c>
@@ -7635,7 +7635,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>170</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>170</v>
       </c>
@@ -7712,7 +7712,7 @@
       </c>
       <c r="M102" s="5"/>
     </row>
-    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>170</v>
       </c>
@@ -7753,7 +7753,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>170</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>170</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>170</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="107" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>170</v>
       </c>
@@ -7911,7 +7911,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>170</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>170</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>170</v>
       </c>
@@ -8034,7 +8034,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>170</v>
       </c>
@@ -8072,7 +8072,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="112" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>170</v>
       </c>
@@ -8111,7 +8111,7 @@
       </c>
       <c r="M112" s="5"/>
     </row>
-    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>170</v>
       </c>
@@ -8140,7 +8140,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>205</v>
       </c>
@@ -8181,7 +8181,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>205</v>
       </c>
@@ -8222,7 +8222,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>205</v>
       </c>
@@ -8263,7 +8263,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>205</v>
       </c>
@@ -8301,7 +8301,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="118" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>205</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>205</v>
       </c>
@@ -8378,7 +8378,7 @@
       </c>
       <c r="M119" s="4"/>
     </row>
-    <row r="120" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>205</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>205</v>
       </c>
@@ -8457,7 +8457,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>205</v>
       </c>
@@ -8498,7 +8498,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>205</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>205</v>
       </c>
@@ -8578,7 +8578,7 @@
       </c>
       <c r="M124" s="4"/>
     </row>
-    <row r="125" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>205</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>205</v>
       </c>
@@ -8655,7 +8655,7 @@
       </c>
       <c r="M126" s="4"/>
     </row>
-    <row r="127" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>205</v>
       </c>
@@ -8693,7 +8693,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>205</v>
       </c>
@@ -8734,7 +8734,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>205</v>
       </c>
@@ -8775,7 +8775,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>205</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>205</v>
       </c>
@@ -8854,7 +8854,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="132" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>205</v>
       </c>
@@ -8892,7 +8892,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>205</v>
       </c>
@@ -8930,7 +8930,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="134" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>205</v>
       </c>
@@ -8969,7 +8969,7 @@
       </c>
       <c r="M134" s="5"/>
     </row>
-    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>205</v>
       </c>
@@ -9010,7 +9010,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>205</v>
       </c>
@@ -9051,7 +9051,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>205</v>
       </c>
@@ -9092,7 +9092,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>205</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="139" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>205</v>
       </c>
@@ -9169,7 +9169,7 @@
       </c>
       <c r="M139" s="5"/>
     </row>
-    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>205</v>
       </c>
@@ -9207,7 +9207,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="141" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>205</v>
       </c>
@@ -9246,7 +9246,7 @@
       </c>
       <c r="M141" s="5"/>
     </row>
-    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>246</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>246</v>
       </c>
@@ -9322,7 +9322,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>246</v>
       </c>
@@ -9360,7 +9360,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>246</v>
       </c>
@@ -9398,7 +9398,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>246</v>
       </c>
@@ -9436,7 +9436,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>246</v>
       </c>
@@ -9474,7 +9474,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>246</v>
       </c>
@@ -9509,7 +9509,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>246</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>246</v>
       </c>
@@ -9591,7 +9591,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>246</v>
       </c>
@@ -9632,7 +9632,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>246</v>
       </c>
@@ -9670,7 +9670,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>246</v>
       </c>
@@ -9711,7 +9711,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>246</v>
       </c>
@@ -9746,7 +9746,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>246</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>246</v>
       </c>
@@ -9816,7 +9816,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>246</v>
       </c>
@@ -9857,7 +9857,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>246</v>
       </c>
@@ -9898,7 +9898,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>246</v>
       </c>
@@ -9939,7 +9939,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>246</v>
       </c>
@@ -9978,7 +9978,7 @@
       </c>
       <c r="M160" s="4"/>
     </row>
-    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>246</v>
       </c>
@@ -10019,7 +10019,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>246</v>
       </c>
@@ -10054,7 +10054,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>246</v>
       </c>
@@ -10089,7 +10089,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>246</v>
       </c>
@@ -10126,7 +10126,7 @@
       </c>
       <c r="M164" s="4"/>
     </row>
-    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>246</v>
       </c>
@@ -10167,7 +10167,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>246</v>
       </c>
@@ -10208,7 +10208,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>246</v>
       </c>
@@ -10249,7 +10249,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>246</v>
       </c>
@@ -10288,7 +10288,7 @@
       </c>
       <c r="M168" s="4"/>
     </row>
-    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>246</v>
       </c>
@@ -10329,7 +10329,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>246</v>
       </c>
@@ -10364,7 +10364,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>246</v>
       </c>
@@ -10399,7 +10399,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>246</v>
       </c>
@@ -10436,7 +10436,7 @@
       </c>
       <c r="M172" s="4"/>
     </row>
-    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>246</v>
       </c>
@@ -10477,7 +10477,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>246</v>
       </c>
@@ -10518,7 +10518,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>246</v>
       </c>
@@ -10559,7 +10559,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>246</v>
       </c>
@@ -10598,7 +10598,7 @@
       </c>
       <c r="M176" s="4"/>
     </row>
-    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>246</v>
       </c>
@@ -10639,7 +10639,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>246</v>
       </c>
@@ -10674,7 +10674,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>246</v>
       </c>
@@ -10709,7 +10709,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>246</v>
       </c>
@@ -10746,7 +10746,7 @@
       </c>
       <c r="M180" s="4"/>
     </row>
-    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>246</v>
       </c>
@@ -10787,7 +10787,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
         <v>246</v>
       </c>
@@ -10828,7 +10828,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>246</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
         <v>246</v>
       </c>
@@ -10908,7 +10908,7 @@
       </c>
       <c r="M184" s="4"/>
     </row>
-    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>246</v>
       </c>
@@ -10949,7 +10949,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>246</v>
       </c>
@@ -10984,7 +10984,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>246</v>
       </c>
@@ -11019,7 +11019,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="188" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>330</v>
       </c>
@@ -11048,7 +11048,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="189" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
         <v>330</v>
       </c>
@@ -11081,7 +11081,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>64</v>
       </c>
@@ -11119,7 +11119,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>64</v>
       </c>
@@ -11157,7 +11157,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>345</v>
       </c>
@@ -11183,7 +11183,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="193" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>345</v>
       </c>
@@ -11212,7 +11212,7 @@
       </c>
       <c r="M193" s="5"/>
     </row>
-    <row r="194" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>345</v>
       </c>
@@ -11239,7 +11239,7 @@
       <c r="L194" s="5"/>
       <c r="M194" s="5"/>
     </row>
-    <row r="195" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>345</v>
       </c>
@@ -11264,7 +11264,7 @@
       <c r="L195" s="5"/>
       <c r="M195" s="5"/>
     </row>
-    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>8</v>
       </c>
@@ -11303,7 +11303,7 @@
       </c>
       <c r="M196" s="4"/>
     </row>
-    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
         <v>8</v>
       </c>
@@ -11342,7 +11342,7 @@
       </c>
       <c r="M197" s="4"/>
     </row>
-    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>8</v>
       </c>
@@ -11380,7 +11380,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="199" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>170</v>
       </c>
@@ -11418,7 +11418,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="200" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>170</v>
       </c>
@@ -11457,7 +11457,7 @@
       </c>
       <c r="M200" s="5"/>
     </row>
-    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>170</v>
       </c>
@@ -11495,7 +11495,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="202" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>170</v>
       </c>
@@ -11533,7 +11533,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="203" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>170</v>
       </c>
@@ -11571,7 +11571,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="204" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>170</v>
       </c>
@@ -11609,7 +11609,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="205" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>170</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="206" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>170</v>
       </c>
@@ -11686,7 +11686,7 @@
       </c>
       <c r="M206" s="5"/>
     </row>
-    <row r="207" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>170</v>
       </c>
@@ -11724,7 +11724,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="208" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>170</v>
       </c>
@@ -11763,7 +11763,7 @@
       </c>
       <c r="M208" s="5"/>
     </row>
-    <row r="209" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>170</v>
       </c>
@@ -11801,7 +11801,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="210" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>170</v>
       </c>
@@ -11840,7 +11840,7 @@
       </c>
       <c r="M210" s="5"/>
     </row>
-    <row r="211" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>380</v>
       </c>
@@ -11879,7 +11879,7 @@
       </c>
       <c r="M211" s="4"/>
     </row>
-    <row r="212" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>380</v>
       </c>
@@ -11917,7 +11917,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="213" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>380</v>
       </c>
@@ -11956,7 +11956,7 @@
       </c>
       <c r="M213" s="4"/>
     </row>
-    <row r="214" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>380</v>
       </c>
@@ -11994,7 +11994,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="215" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>380</v>
       </c>
@@ -12035,7 +12035,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="216" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>380</v>
       </c>
@@ -12076,7 +12076,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="217" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>380</v>
       </c>
@@ -12117,7 +12117,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="218" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>380</v>
       </c>
@@ -12158,7 +12158,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="219" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>380</v>
       </c>
@@ -12199,7 +12199,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="220" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>380</v>
       </c>
@@ -12240,7 +12240,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="221" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>380</v>
       </c>
@@ -12278,7 +12278,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="222" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>380</v>
       </c>
@@ -12316,7 +12316,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="223" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>380</v>
       </c>
@@ -12354,7 +12354,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="224" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>380</v>
       </c>
@@ -12392,7 +12392,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="225" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>380</v>
       </c>
@@ -12430,7 +12430,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="226" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>380</v>
       </c>
@@ -12468,7 +12468,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="227" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>380</v>
       </c>
@@ -12506,7 +12506,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="228" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>380</v>
       </c>
@@ -12544,7 +12544,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="229" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>380</v>
       </c>
@@ -12585,7 +12585,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="230" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>380</v>
       </c>
@@ -12626,7 +12626,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="231" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>380</v>
       </c>
@@ -12667,7 +12667,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="232" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>380</v>
       </c>
@@ -12708,7 +12708,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="233" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>380</v>
       </c>
@@ -12749,7 +12749,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="234" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>380</v>
       </c>
@@ -12790,7 +12790,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="235" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>8</v>
       </c>
@@ -12828,7 +12828,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="236" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>8</v>
       </c>
@@ -12866,7 +12866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="237" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>330</v>
       </c>
@@ -12894,15 +12894,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M237" xr:uid="{18737FC4-8F93-4286-8DA0-398B4A1B23DB}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Vertical Composition"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="forest_calcs.TPA_BA_QMDBH_Plot &amp; Level"/>
-      </filters>
+    <filterColumn colId="1">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12919,19 +12912,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="32.26953125" customWidth="1"/>
-    <col min="6" max="6" width="33.453125" customWidth="1"/>
-    <col min="7" max="7" width="31.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12957,12 +12950,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>496</v>
       </c>

</xml_diff>